<commit_message>
se agrega frontend con backend
</commit_message>
<xml_diff>
--- a/EduMultiPro 2 Parte/2-Normalizacion 3FN/Normalizacion.xlsx
+++ b/EduMultiPro 2 Parte/2-Normalizacion 3FN/Normalizacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\EduMultiPro\EduMultiPro 2 Parte\2-Normalizacion 3FN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87F9AF2-3FBD-4BA4-8BD8-0790C3F1CD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174A9CFE-4B08-4354-9B4B-0DAF01682AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="380">
   <si>
     <t>Nombre</t>
   </si>
@@ -1151,6 +1151,18 @@
   </si>
   <si>
     <t>oso123</t>
+  </si>
+  <si>
+    <t>Descripcion2</t>
+  </si>
+  <si>
+    <t>Descripcion3</t>
+  </si>
+  <si>
+    <t>Descripcion1</t>
+  </si>
+  <si>
+    <t>Encabezado</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1284,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1300,6 +1312,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1477,7 +1495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1930,26 +1948,482 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="752">
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
+  <dxfs count="759">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="d/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1960,12 +2434,8 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2564,84 +3034,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <top style="thin">
           <color indexed="64"/>
@@ -3752,214 +4144,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -7666,6 +7850,29 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -13117,6 +13324,15 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -18514,79 +18730,79 @@
   </dxfs>
   <tableStyles count="15">
     <tableStyle name="Hoja 1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="751"/>
-      <tableStyleElement type="firstRowStripe" dxfId="750"/>
-      <tableStyleElement type="secondRowStripe" dxfId="749"/>
+      <tableStyleElement type="headerRow" dxfId="758"/>
+      <tableStyleElement type="firstRowStripe" dxfId="757"/>
+      <tableStyleElement type="secondRowStripe" dxfId="756"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
-      <tableStyleElement type="headerRow" dxfId="748"/>
-      <tableStyleElement type="firstRowStripe" dxfId="747"/>
-      <tableStyleElement type="secondRowStripe" dxfId="746"/>
+      <tableStyleElement type="headerRow" dxfId="755"/>
+      <tableStyleElement type="firstRowStripe" dxfId="754"/>
+      <tableStyleElement type="secondRowStripe" dxfId="753"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
-      <tableStyleElement type="headerRow" dxfId="745"/>
-      <tableStyleElement type="firstRowStripe" dxfId="744"/>
-      <tableStyleElement type="secondRowStripe" dxfId="743"/>
+      <tableStyleElement type="headerRow" dxfId="752"/>
+      <tableStyleElement type="firstRowStripe" dxfId="751"/>
+      <tableStyleElement type="secondRowStripe" dxfId="750"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 4" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF03000000}">
-      <tableStyleElement type="headerRow" dxfId="742"/>
-      <tableStyleElement type="firstRowStripe" dxfId="741"/>
-      <tableStyleElement type="secondRowStripe" dxfId="740"/>
+      <tableStyleElement type="headerRow" dxfId="749"/>
+      <tableStyleElement type="firstRowStripe" dxfId="748"/>
+      <tableStyleElement type="secondRowStripe" dxfId="747"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 5" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF04000000}">
-      <tableStyleElement type="headerRow" dxfId="739"/>
-      <tableStyleElement type="firstRowStripe" dxfId="738"/>
-      <tableStyleElement type="secondRowStripe" dxfId="737"/>
+      <tableStyleElement type="headerRow" dxfId="746"/>
+      <tableStyleElement type="firstRowStripe" dxfId="745"/>
+      <tableStyleElement type="secondRowStripe" dxfId="744"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 6" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF05000000}">
-      <tableStyleElement type="headerRow" dxfId="736"/>
-      <tableStyleElement type="firstRowStripe" dxfId="735"/>
-      <tableStyleElement type="secondRowStripe" dxfId="734"/>
+      <tableStyleElement type="headerRow" dxfId="743"/>
+      <tableStyleElement type="firstRowStripe" dxfId="742"/>
+      <tableStyleElement type="secondRowStripe" dxfId="741"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 7" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF06000000}">
-      <tableStyleElement type="headerRow" dxfId="733"/>
-      <tableStyleElement type="firstRowStripe" dxfId="732"/>
-      <tableStyleElement type="secondRowStripe" dxfId="731"/>
+      <tableStyleElement type="headerRow" dxfId="740"/>
+      <tableStyleElement type="firstRowStripe" dxfId="739"/>
+      <tableStyleElement type="secondRowStripe" dxfId="738"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 8" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF07000000}">
-      <tableStyleElement type="headerRow" dxfId="730"/>
-      <tableStyleElement type="firstRowStripe" dxfId="729"/>
-      <tableStyleElement type="secondRowStripe" dxfId="728"/>
+      <tableStyleElement type="headerRow" dxfId="737"/>
+      <tableStyleElement type="firstRowStripe" dxfId="736"/>
+      <tableStyleElement type="secondRowStripe" dxfId="735"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 9" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF08000000}">
-      <tableStyleElement type="headerRow" dxfId="727"/>
-      <tableStyleElement type="firstRowStripe" dxfId="726"/>
-      <tableStyleElement type="secondRowStripe" dxfId="725"/>
+      <tableStyleElement type="headerRow" dxfId="734"/>
+      <tableStyleElement type="firstRowStripe" dxfId="733"/>
+      <tableStyleElement type="secondRowStripe" dxfId="732"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 10" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF09000000}">
-      <tableStyleElement type="headerRow" dxfId="724"/>
-      <tableStyleElement type="firstRowStripe" dxfId="723"/>
-      <tableStyleElement type="secondRowStripe" dxfId="722"/>
+      <tableStyleElement type="headerRow" dxfId="731"/>
+      <tableStyleElement type="firstRowStripe" dxfId="730"/>
+      <tableStyleElement type="secondRowStripe" dxfId="729"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 11" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0A000000}">
-      <tableStyleElement type="headerRow" dxfId="721"/>
-      <tableStyleElement type="firstRowStripe" dxfId="720"/>
-      <tableStyleElement type="secondRowStripe" dxfId="719"/>
+      <tableStyleElement type="headerRow" dxfId="728"/>
+      <tableStyleElement type="firstRowStripe" dxfId="727"/>
+      <tableStyleElement type="secondRowStripe" dxfId="726"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 12" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0B000000}">
-      <tableStyleElement type="headerRow" dxfId="718"/>
-      <tableStyleElement type="firstRowStripe" dxfId="717"/>
-      <tableStyleElement type="secondRowStripe" dxfId="716"/>
+      <tableStyleElement type="headerRow" dxfId="725"/>
+      <tableStyleElement type="firstRowStripe" dxfId="724"/>
+      <tableStyleElement type="secondRowStripe" dxfId="723"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 13" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0C000000}">
-      <tableStyleElement type="headerRow" dxfId="715"/>
-      <tableStyleElement type="firstRowStripe" dxfId="714"/>
-      <tableStyleElement type="secondRowStripe" dxfId="713"/>
+      <tableStyleElement type="headerRow" dxfId="722"/>
+      <tableStyleElement type="firstRowStripe" dxfId="721"/>
+      <tableStyleElement type="secondRowStripe" dxfId="720"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 14" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0D000000}">
-      <tableStyleElement type="headerRow" dxfId="712"/>
-      <tableStyleElement type="firstRowStripe" dxfId="711"/>
-      <tableStyleElement type="secondRowStripe" dxfId="710"/>
+      <tableStyleElement type="headerRow" dxfId="719"/>
+      <tableStyleElement type="firstRowStripe" dxfId="718"/>
+      <tableStyleElement type="secondRowStripe" dxfId="717"/>
     </tableStyle>
     <tableStyle name="Hoja 1-style 15" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF0E000000}">
-      <tableStyleElement type="headerRow" dxfId="709"/>
-      <tableStyleElement type="firstRowStripe" dxfId="708"/>
-      <tableStyleElement type="secondRowStripe" dxfId="707"/>
+      <tableStyleElement type="headerRow" dxfId="716"/>
+      <tableStyleElement type="firstRowStripe" dxfId="715"/>
+      <tableStyleElement type="secondRowStripe" dxfId="714"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -18601,1049 +18817,1061 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{32320B99-21E0-465A-836A-F8A08214D8FE}" name="Tabla16" displayName="Tabla16" ref="B3:N6" totalsRowShown="0" headerRowDxfId="706" dataDxfId="704" headerRowBorderDxfId="705" tableBorderDxfId="703" totalsRowBorderDxfId="702">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{32320B99-21E0-465A-836A-F8A08214D8FE}" name="Tabla16" displayName="Tabla16" ref="B3:N6" totalsRowShown="0" headerRowDxfId="713" dataDxfId="711" headerRowBorderDxfId="712" tableBorderDxfId="710" totalsRowBorderDxfId="709">
   <autoFilter ref="B3:N6" xr:uid="{32320B99-21E0-465A-836A-F8A08214D8FE}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{4E430143-297C-4B15-AC85-77B5D80FC124}" name="N.O Documento" dataDxfId="701"/>
-    <tableColumn id="2" xr3:uid="{2C57AC1C-117E-4A7A-A04D-8BC7BBB5C2EB}" name="Nombres" dataDxfId="700"/>
-    <tableColumn id="3" xr3:uid="{5FCCAC06-E191-41B9-B824-2BB554A1097F}" name="Apellidos" dataDxfId="699"/>
-    <tableColumn id="4" xr3:uid="{75E21A5A-F49E-4818-B618-950A37714EF7}" name="Tipo Documento" dataDxfId="698"/>
-    <tableColumn id="5" xr3:uid="{A057F466-7DAC-4A37-8240-FB9E5FB1FBFA}" name="Correo1" dataDxfId="697"/>
-    <tableColumn id="6" xr3:uid="{176DE0F0-8E2F-41D9-9C48-807AA1DBC8E2}" name="Correo 2" dataDxfId="696"/>
-    <tableColumn id="7" xr3:uid="{F64A4E6B-1D94-4898-A00C-A652268A0C4B}" name="Contactos" dataDxfId="695"/>
-    <tableColumn id="8" xr3:uid="{87CA0814-F735-4EA0-AB02-3D1AA2281A06}" name="Rol" dataDxfId="694"/>
-    <tableColumn id="9" xr3:uid="{BB4AB0FA-C9FE-4F90-81AE-9D7A8BF7CC51}" name="Fecha Nacimiento" dataDxfId="693"/>
-    <tableColumn id="10" xr3:uid="{268CE79E-176D-41BB-A7D9-D0AB1CBC4964}" name="Horario" dataDxfId="692"/>
-    <tableColumn id="11" xr3:uid="{AA52A32C-793A-4C29-ABF0-9156F1760E5B}" name="Cursos" dataDxfId="691"/>
-    <tableColumn id="12" xr3:uid="{D74C05D9-332B-44AE-8ADC-1178D2C812AA}" name="Jornada" dataDxfId="690"/>
-    <tableColumn id="13" xr3:uid="{070EE2F1-C7DE-4EA5-9DAE-1B8A9DF3D740}" name="Grado" dataDxfId="689"/>
+    <tableColumn id="1" xr3:uid="{4E430143-297C-4B15-AC85-77B5D80FC124}" name="N.O Documento" dataDxfId="708"/>
+    <tableColumn id="2" xr3:uid="{2C57AC1C-117E-4A7A-A04D-8BC7BBB5C2EB}" name="Nombres" dataDxfId="707"/>
+    <tableColumn id="3" xr3:uid="{5FCCAC06-E191-41B9-B824-2BB554A1097F}" name="Apellidos" dataDxfId="706"/>
+    <tableColumn id="4" xr3:uid="{75E21A5A-F49E-4818-B618-950A37714EF7}" name="Tipo Documento" dataDxfId="705"/>
+    <tableColumn id="5" xr3:uid="{A057F466-7DAC-4A37-8240-FB9E5FB1FBFA}" name="Correo1" dataDxfId="704"/>
+    <tableColumn id="6" xr3:uid="{176DE0F0-8E2F-41D9-9C48-807AA1DBC8E2}" name="Correo 2" dataDxfId="703"/>
+    <tableColumn id="7" xr3:uid="{F64A4E6B-1D94-4898-A00C-A652268A0C4B}" name="Contactos" dataDxfId="702"/>
+    <tableColumn id="8" xr3:uid="{87CA0814-F735-4EA0-AB02-3D1AA2281A06}" name="Rol" dataDxfId="701"/>
+    <tableColumn id="9" xr3:uid="{BB4AB0FA-C9FE-4F90-81AE-9D7A8BF7CC51}" name="Fecha Nacimiento" dataDxfId="700"/>
+    <tableColumn id="10" xr3:uid="{268CE79E-176D-41BB-A7D9-D0AB1CBC4964}" name="Horario" dataDxfId="699"/>
+    <tableColumn id="11" xr3:uid="{AA52A32C-793A-4C29-ABF0-9156F1760E5B}" name="Cursos" dataDxfId="698"/>
+    <tableColumn id="12" xr3:uid="{D74C05D9-332B-44AE-8ADC-1178D2C812AA}" name="Jornada" dataDxfId="697"/>
+    <tableColumn id="13" xr3:uid="{070EE2F1-C7DE-4EA5-9DAE-1B8A9DF3D740}" name="Grado" dataDxfId="696"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{25CE9884-E391-4CC6-AE7A-906849F7DA66}" name="Tabla25" displayName="Tabla25" ref="B33:R36" totalsRowShown="0" headerRowDxfId="582" dataDxfId="580" headerRowBorderDxfId="581" tableBorderDxfId="579" totalsRowBorderDxfId="578">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="25" xr:uid="{25CE9884-E391-4CC6-AE7A-906849F7DA66}" name="Tabla25" displayName="Tabla25" ref="B33:R36" totalsRowShown="0" headerRowDxfId="589" dataDxfId="587" headerRowBorderDxfId="588" tableBorderDxfId="586" totalsRowBorderDxfId="585">
   <autoFilter ref="B33:R36" xr:uid="{25CE9884-E391-4CC6-AE7A-906849F7DA66}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{C1CB3A6B-7355-4B8D-836D-885E5241993D}" name="ID Boletin" dataDxfId="577"/>
-    <tableColumn id="2" xr3:uid="{A3722960-E3F7-4800-BA86-F88A210C5CB2}" name="Nombre " dataDxfId="576"/>
-    <tableColumn id="3" xr3:uid="{7E35413E-AD9B-4AD9-AAD3-978979D010BD}" name="Institucion" dataDxfId="575"/>
-    <tableColumn id="4" xr3:uid="{ABDF3F44-65E5-414B-8EEA-4F7EFB698717}" name="Sede" dataDxfId="574"/>
-    <tableColumn id="5" xr3:uid="{2B3D944D-FAF8-4F7B-A6C8-4703FB78DD17}" name="Año" dataDxfId="573"/>
-    <tableColumn id="6" xr3:uid="{EDBB2B97-9F59-49B0-B363-CA00BDFD1300}" name="Resolucion" dataDxfId="572"/>
-    <tableColumn id="7" xr3:uid="{7AECAD09-A0A0-4AB5-B398-BD5BE2272EF2}" name="ID Jornada" dataDxfId="571"/>
-    <tableColumn id="8" xr3:uid="{8CCD0E62-C9FB-419B-887D-C02CB4D35383}" name="ID Periodo" dataDxfId="570"/>
-    <tableColumn id="9" xr3:uid="{6C8DE7C3-FEE9-4A39-AF2E-FE356DA2C487}" name="ID Curso" dataDxfId="569"/>
-    <tableColumn id="10" xr3:uid="{5A1554C7-BBF0-4E32-AD3C-463FC01E1EEA}" name="ID Profesor" dataDxfId="568"/>
-    <tableColumn id="11" xr3:uid="{D537ADB7-CFE0-46D8-9282-67DFDF056BF0}" name="ID Nota Final" dataDxfId="567"/>
-    <tableColumn id="12" xr3:uid="{58BAE0F7-97F9-4208-84D1-5A367EE91AC8}" name="Fallas " dataDxfId="566"/>
-    <tableColumn id="13" xr3:uid="{1DCBC03B-2E6A-4755-B0A7-CFA225399BA9}" name="Observaciones" dataDxfId="565"/>
-    <tableColumn id="14" xr3:uid="{A6873FBA-F1C2-4F60-8D9A-BF4C24CDBD38}" name="Estudiante" dataDxfId="564"/>
-    <tableColumn id="15" xr3:uid="{AF82CDF5-BEA9-4934-83DC-962125D6F31E}" name="Puesto" dataDxfId="563"/>
-    <tableColumn id="16" xr3:uid="{E4527C9A-D349-469D-B6B3-51214007816D}" name="ID Valoracion" dataDxfId="562"/>
-    <tableColumn id="17" xr3:uid="{8838E87D-4FC3-403C-A8D3-49EF7FFC38A9}" name="Comportamiento" dataDxfId="561"/>
+    <tableColumn id="1" xr3:uid="{C1CB3A6B-7355-4B8D-836D-885E5241993D}" name="ID Boletin" dataDxfId="584"/>
+    <tableColumn id="2" xr3:uid="{A3722960-E3F7-4800-BA86-F88A210C5CB2}" name="Nombre " dataDxfId="583"/>
+    <tableColumn id="3" xr3:uid="{7E35413E-AD9B-4AD9-AAD3-978979D010BD}" name="Institucion" dataDxfId="582"/>
+    <tableColumn id="4" xr3:uid="{ABDF3F44-65E5-414B-8EEA-4F7EFB698717}" name="Sede" dataDxfId="581"/>
+    <tableColumn id="5" xr3:uid="{2B3D944D-FAF8-4F7B-A6C8-4703FB78DD17}" name="Año" dataDxfId="580"/>
+    <tableColumn id="6" xr3:uid="{EDBB2B97-9F59-49B0-B363-CA00BDFD1300}" name="Resolucion" dataDxfId="579"/>
+    <tableColumn id="7" xr3:uid="{7AECAD09-A0A0-4AB5-B398-BD5BE2272EF2}" name="ID Jornada" dataDxfId="578"/>
+    <tableColumn id="8" xr3:uid="{8CCD0E62-C9FB-419B-887D-C02CB4D35383}" name="ID Periodo" dataDxfId="577"/>
+    <tableColumn id="9" xr3:uid="{6C8DE7C3-FEE9-4A39-AF2E-FE356DA2C487}" name="ID Curso" dataDxfId="576"/>
+    <tableColumn id="10" xr3:uid="{5A1554C7-BBF0-4E32-AD3C-463FC01E1EEA}" name="ID Profesor" dataDxfId="575"/>
+    <tableColumn id="11" xr3:uid="{D537ADB7-CFE0-46D8-9282-67DFDF056BF0}" name="ID Nota Final" dataDxfId="574"/>
+    <tableColumn id="12" xr3:uid="{58BAE0F7-97F9-4208-84D1-5A367EE91AC8}" name="Fallas " dataDxfId="573"/>
+    <tableColumn id="13" xr3:uid="{1DCBC03B-2E6A-4755-B0A7-CFA225399BA9}" name="Observaciones" dataDxfId="572"/>
+    <tableColumn id="14" xr3:uid="{A6873FBA-F1C2-4F60-8D9A-BF4C24CDBD38}" name="Estudiante" dataDxfId="571"/>
+    <tableColumn id="15" xr3:uid="{AF82CDF5-BEA9-4934-83DC-962125D6F31E}" name="Puesto" dataDxfId="570"/>
+    <tableColumn id="16" xr3:uid="{E4527C9A-D349-469D-B6B3-51214007816D}" name="ID Valoracion" dataDxfId="569"/>
+    <tableColumn id="17" xr3:uid="{8838E87D-4FC3-403C-A8D3-49EF7FFC38A9}" name="Comportamiento" dataDxfId="568"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{5ACE0EB5-BF41-4D03-A01D-DBE050CCB9FB}" name="Tabla1927" displayName="Tabla1927" ref="B40:I43" totalsRowShown="0" headerRowDxfId="560" dataDxfId="558" headerRowBorderDxfId="559" tableBorderDxfId="557" totalsRowBorderDxfId="556">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{5ACE0EB5-BF41-4D03-A01D-DBE050CCB9FB}" name="Tabla1927" displayName="Tabla1927" ref="B40:I43" totalsRowShown="0" headerRowDxfId="567" dataDxfId="565" headerRowBorderDxfId="566" tableBorderDxfId="564" totalsRowBorderDxfId="563">
   <autoFilter ref="B40:I43" xr:uid="{5ACE0EB5-BF41-4D03-A01D-DBE050CCB9FB}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{8D64FFD6-E265-4FAC-861B-59255CB86913}" name="ID Noticias" dataDxfId="555"/>
-    <tableColumn id="2" xr3:uid="{E5438A13-E581-4F94-A6AF-56C0326A1CEE}" name="Titulo" dataDxfId="554"/>
-    <tableColumn id="3" xr3:uid="{5456FAA0-D014-47B6-84C6-F0F2174C2319}" name="Descripcion" dataDxfId="553"/>
-    <tableColumn id="4" xr3:uid="{EDA54D2F-3416-4B05-9B20-2451921B6049}" name="Fecha" dataDxfId="552"/>
-    <tableColumn id="5" xr3:uid="{9E26D400-BFC4-4A32-8E07-71552A891CD9}" name="Tipo" dataDxfId="551"/>
-    <tableColumn id="6" xr3:uid="{C96DA585-DE91-4E54-A3CA-6F869E91E286}" name="Imagen 1" dataDxfId="550"/>
-    <tableColumn id="7" xr3:uid="{B1FC5614-588F-47FE-8F45-8C4AB8081480}" name="Imagen 2" dataDxfId="549"/>
-    <tableColumn id="8" xr3:uid="{7DAD316D-DF97-49F5-A387-DB4BD20F2785}" name="Imagen 3" dataDxfId="548"/>
+    <tableColumn id="1" xr3:uid="{8D64FFD6-E265-4FAC-861B-59255CB86913}" name="ID Noticias" dataDxfId="562"/>
+    <tableColumn id="2" xr3:uid="{E5438A13-E581-4F94-A6AF-56C0326A1CEE}" name="Titulo" dataDxfId="561"/>
+    <tableColumn id="3" xr3:uid="{5456FAA0-D014-47B6-84C6-F0F2174C2319}" name="Descripcion" dataDxfId="560"/>
+    <tableColumn id="4" xr3:uid="{EDA54D2F-3416-4B05-9B20-2451921B6049}" name="Fecha" dataDxfId="559"/>
+    <tableColumn id="5" xr3:uid="{9E26D400-BFC4-4A32-8E07-71552A891CD9}" name="Tipo" dataDxfId="558"/>
+    <tableColumn id="6" xr3:uid="{C96DA585-DE91-4E54-A3CA-6F869E91E286}" name="Imagen 1" dataDxfId="557"/>
+    <tableColumn id="7" xr3:uid="{B1FC5614-588F-47FE-8F45-8C4AB8081480}" name="Imagen 2" dataDxfId="556"/>
+    <tableColumn id="8" xr3:uid="{7DAD316D-DF97-49F5-A387-DB4BD20F2785}" name="Imagen 3" dataDxfId="555"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{22E5DE62-B9DC-4C25-819B-D3B018AF9B78}" name="Tabla27" displayName="Tabla27" ref="Q12:R15" totalsRowShown="0" headerRowDxfId="547" dataDxfId="545" headerRowBorderDxfId="546" tableBorderDxfId="544" totalsRowBorderDxfId="543">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="27" xr:uid="{22E5DE62-B9DC-4C25-819B-D3B018AF9B78}" name="Tabla27" displayName="Tabla27" ref="Q12:R15" totalsRowShown="0" headerRowDxfId="554" dataDxfId="552" headerRowBorderDxfId="553" tableBorderDxfId="551" totalsRowBorderDxfId="550">
   <autoFilter ref="Q12:R15" xr:uid="{22E5DE62-B9DC-4C25-819B-D3B018AF9B78}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3741159B-F11E-49DB-946D-94FBD0D918A2}" name="ID Documento" dataDxfId="542"/>
-    <tableColumn id="2" xr3:uid="{504028F9-5B2C-4DE2-A190-4B3305FE5B05}" name="Tipo Documento" dataDxfId="541"/>
+    <tableColumn id="1" xr3:uid="{3741159B-F11E-49DB-946D-94FBD0D918A2}" name="ID Documento" dataDxfId="549"/>
+    <tableColumn id="2" xr3:uid="{504028F9-5B2C-4DE2-A190-4B3305FE5B05}" name="Tipo Documento" dataDxfId="548"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{002874DA-010C-43F9-828E-5FB847008742}" name="Tabla28" displayName="Tabla28" ref="T12:U14" totalsRowShown="0" headerRowDxfId="540" dataDxfId="538" headerRowBorderDxfId="539" tableBorderDxfId="537" totalsRowBorderDxfId="536">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{002874DA-010C-43F9-828E-5FB847008742}" name="Tabla28" displayName="Tabla28" ref="T12:U14" totalsRowShown="0" headerRowDxfId="547" dataDxfId="545" headerRowBorderDxfId="546" tableBorderDxfId="544" totalsRowBorderDxfId="543">
   <autoFilter ref="T12:U14" xr:uid="{002874DA-010C-43F9-828E-5FB847008742}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CD50E275-53A6-4D78-8EEE-E1A47049ACC5}" name="ID Jornada" dataDxfId="535"/>
-    <tableColumn id="2" xr3:uid="{0E6014F8-93BB-4925-B444-067A3A7BF6CF}" name="Jornada" dataDxfId="534"/>
+    <tableColumn id="1" xr3:uid="{CD50E275-53A6-4D78-8EEE-E1A47049ACC5}" name="ID Jornada" dataDxfId="542"/>
+    <tableColumn id="2" xr3:uid="{0E6014F8-93BB-4925-B444-067A3A7BF6CF}" name="Jornada" dataDxfId="541"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{26DA6AF8-BD2E-4B3F-8335-048B0110FBBA}" name="Tabla29" displayName="Tabla29" ref="W12:X15" totalsRowShown="0" headerRowDxfId="533" dataDxfId="531" headerRowBorderDxfId="532" tableBorderDxfId="530" totalsRowBorderDxfId="529">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="29" xr:uid="{26DA6AF8-BD2E-4B3F-8335-048B0110FBBA}" name="Tabla29" displayName="Tabla29" ref="W12:X15" totalsRowShown="0" headerRowDxfId="540" dataDxfId="538" headerRowBorderDxfId="539" tableBorderDxfId="537" totalsRowBorderDxfId="536">
   <autoFilter ref="W12:X15" xr:uid="{26DA6AF8-BD2E-4B3F-8335-048B0110FBBA}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CF81FB27-65E5-4229-8DF6-EC95682F4E29}" name="ID Curso" dataDxfId="528"/>
-    <tableColumn id="2" xr3:uid="{B461E2E8-C7D7-4DCE-B77D-D9F4E5D4823C}" name="Curso" dataDxfId="527"/>
+    <tableColumn id="1" xr3:uid="{CF81FB27-65E5-4229-8DF6-EC95682F4E29}" name="ID Curso" dataDxfId="535"/>
+    <tableColumn id="2" xr3:uid="{B461E2E8-C7D7-4DCE-B77D-D9F4E5D4823C}" name="Curso" dataDxfId="534"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{C9BD62A1-EEDE-40AB-8D21-0258304B86BE}" name="Tabla30" displayName="Tabla30" ref="W5:X8" totalsRowShown="0" headerRowDxfId="526" dataDxfId="525">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="30" xr:uid="{C9BD62A1-EEDE-40AB-8D21-0258304B86BE}" name="Tabla30" displayName="Tabla30" ref="W5:X8" totalsRowShown="0" headerRowDxfId="533" dataDxfId="532">
   <autoFilter ref="W5:X8" xr:uid="{C9BD62A1-EEDE-40AB-8D21-0258304B86BE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{158F37AC-4571-4B92-9D34-58AEACB896FC}" name="ID Grado" dataDxfId="524"/>
-    <tableColumn id="2" xr3:uid="{3FBF9672-BDF1-4E1D-8C58-FD6F081328B8}" name="Grado" dataDxfId="523"/>
+    <tableColumn id="1" xr3:uid="{158F37AC-4571-4B92-9D34-58AEACB896FC}" name="ID Grado" dataDxfId="531"/>
+    <tableColumn id="2" xr3:uid="{3FBF9672-BDF1-4E1D-8C58-FD6F081328B8}" name="Grado" dataDxfId="530"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{57E541AC-F315-4FBC-B506-12A4565DA410}" name="Tabla31" displayName="Tabla31" ref="I26:J30" totalsRowShown="0" headerRowDxfId="522" dataDxfId="520" headerRowBorderDxfId="521" tableBorderDxfId="519" totalsRowBorderDxfId="518">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="31" xr:uid="{57E541AC-F315-4FBC-B506-12A4565DA410}" name="Tabla31" displayName="Tabla31" ref="I26:J30" totalsRowShown="0" headerRowDxfId="529" dataDxfId="527" headerRowBorderDxfId="528" tableBorderDxfId="526" totalsRowBorderDxfId="525">
   <autoFilter ref="I26:J30" xr:uid="{57E541AC-F315-4FBC-B506-12A4565DA410}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{924A6F13-5BA7-4B83-8AF5-11B0D955AE26}" name="ID Perido" dataDxfId="517"/>
-    <tableColumn id="2" xr3:uid="{81F629A1-CD62-437D-9560-A1ACAE680132}" name="Periodo" dataDxfId="516"/>
+    <tableColumn id="1" xr3:uid="{924A6F13-5BA7-4B83-8AF5-11B0D955AE26}" name="ID Perido" dataDxfId="524"/>
+    <tableColumn id="2" xr3:uid="{81F629A1-CD62-437D-9560-A1ACAE680132}" name="Periodo" dataDxfId="523"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{8AA9B5A0-8D0A-4B5D-96CD-5F2A70320C49}" name="Tabla33" displayName="Tabla33" ref="Q40:R44" totalsRowShown="0" headerRowDxfId="515" dataDxfId="513" headerRowBorderDxfId="514" tableBorderDxfId="512" totalsRowBorderDxfId="511">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="33" xr:uid="{8AA9B5A0-8D0A-4B5D-96CD-5F2A70320C49}" name="Tabla33" displayName="Tabla33" ref="Q40:R44" totalsRowShown="0" headerRowDxfId="522" dataDxfId="520" headerRowBorderDxfId="521" tableBorderDxfId="519" totalsRowBorderDxfId="518">
   <autoFilter ref="Q40:R44" xr:uid="{8AA9B5A0-8D0A-4B5D-96CD-5F2A70320C49}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{B8391C68-B573-4E29-9392-8A2C45ED60E6}" name="ID Valoracion" dataDxfId="510"/>
-    <tableColumn id="2" xr3:uid="{4E94EAAC-A346-4F46-B312-445764517E1F}" name="Valoracion" dataDxfId="509"/>
+    <tableColumn id="1" xr3:uid="{B8391C68-B573-4E29-9392-8A2C45ED60E6}" name="ID Valoracion" dataDxfId="517"/>
+    <tableColumn id="2" xr3:uid="{4E94EAAC-A346-4F46-B312-445764517E1F}" name="Valoracion" dataDxfId="516"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{4550AE0F-9688-48E0-A9A8-AADC2926F0DC}" name="Tabla34" displayName="Tabla34" ref="Z5:AA9" totalsRowShown="0" headerRowDxfId="508" dataDxfId="506" headerRowBorderDxfId="507" tableBorderDxfId="505" totalsRowBorderDxfId="504">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{4550AE0F-9688-48E0-A9A8-AADC2926F0DC}" name="Tabla34" displayName="Tabla34" ref="Z5:AA9" totalsRowShown="0" headerRowDxfId="515" dataDxfId="513" headerRowBorderDxfId="514" tableBorderDxfId="512" totalsRowBorderDxfId="511">
   <autoFilter ref="Z5:AA9" xr:uid="{4550AE0F-9688-48E0-A9A8-AADC2926F0DC}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C63A4630-CD0E-465B-A3A1-62B9C6CD1F41}" name="ID Rol" dataDxfId="503"/>
-    <tableColumn id="2" xr3:uid="{A255157E-B511-44EB-BEA1-956BB7959E3D}" name="Rol" dataDxfId="502"/>
+    <tableColumn id="1" xr3:uid="{C63A4630-CD0E-465B-A3A1-62B9C6CD1F41}" name="ID Rol" dataDxfId="510"/>
+    <tableColumn id="2" xr3:uid="{A255157E-B511-44EB-BEA1-956BB7959E3D}" name="Rol" dataDxfId="509"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{7F1B6FA1-D40F-4AE4-ADEE-3DD8BCE9B8E0}" name="Tabla35" displayName="Tabla35" ref="Z12:AA15" totalsRowShown="0" headerRowDxfId="501" dataDxfId="499" headerRowBorderDxfId="500" tableBorderDxfId="498" totalsRowBorderDxfId="497">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{7F1B6FA1-D40F-4AE4-ADEE-3DD8BCE9B8E0}" name="Tabla35" displayName="Tabla35" ref="Z12:AA15" totalsRowShown="0" headerRowDxfId="508" dataDxfId="506" headerRowBorderDxfId="507" tableBorderDxfId="505" totalsRowBorderDxfId="504">
   <autoFilter ref="Z12:AA15" xr:uid="{7F1B6FA1-D40F-4AE4-ADEE-3DD8BCE9B8E0}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4CE5D300-4032-4777-9186-AEC3379D0B5B}" name="ID Materia" dataDxfId="496"/>
-    <tableColumn id="2" xr3:uid="{91BE384F-5FA3-4A57-B76A-CFF3455B26FF}" name="Materia" dataDxfId="495"/>
+    <tableColumn id="1" xr3:uid="{4CE5D300-4032-4777-9186-AEC3379D0B5B}" name="ID Materia" dataDxfId="503"/>
+    <tableColumn id="2" xr3:uid="{91BE384F-5FA3-4A57-B76A-CFF3455B26FF}" name="Materia" dataDxfId="502"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{FCF8D94F-AB28-45E3-95FA-DA0A000E517E}" name="Tabla17" displayName="Tabla17" ref="B10:H13" totalsRowShown="0" headerRowDxfId="688" dataDxfId="686" headerRowBorderDxfId="687" tableBorderDxfId="685" totalsRowBorderDxfId="684">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{FCF8D94F-AB28-45E3-95FA-DA0A000E517E}" name="Tabla17" displayName="Tabla17" ref="B10:H13" totalsRowShown="0" headerRowDxfId="695" dataDxfId="693" headerRowBorderDxfId="694" tableBorderDxfId="692" totalsRowBorderDxfId="691">
   <autoFilter ref="B10:H13" xr:uid="{FCF8D94F-AB28-45E3-95FA-DA0A000E517E}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{DAA14EB8-2CD4-47BE-BC0F-B8E7ADF9FE07}" name="Materia" dataDxfId="683"/>
-    <tableColumn id="2" xr3:uid="{4B71F85E-5F8B-4B47-880E-2A51DA12E203}" name="Aula" dataDxfId="682"/>
-    <tableColumn id="3" xr3:uid="{B9953F19-11A6-4D17-855F-B72FABA275E1}" name="Tareas" dataDxfId="681"/>
-    <tableColumn id="4" xr3:uid="{93A48342-846D-4345-B86E-84B03B9F5BE6}" name="Fecha de Entrega" dataDxfId="680"/>
-    <tableColumn id="5" xr3:uid="{A3806AAD-69B1-4B13-B2A6-2DE84CEE378A}" name="Anuncio" dataDxfId="679"/>
-    <tableColumn id="6" xr3:uid="{4DCE34DE-3E87-4BA4-9215-DC8689B0FB1F}" name="Mensaje" dataDxfId="678"/>
-    <tableColumn id="7" xr3:uid="{0F562F09-3842-4B56-A51E-DF3582B3119D}" name="Nota" dataDxfId="677"/>
+    <tableColumn id="1" xr3:uid="{DAA14EB8-2CD4-47BE-BC0F-B8E7ADF9FE07}" name="Materia" dataDxfId="690"/>
+    <tableColumn id="2" xr3:uid="{4B71F85E-5F8B-4B47-880E-2A51DA12E203}" name="Aula" dataDxfId="689"/>
+    <tableColumn id="3" xr3:uid="{B9953F19-11A6-4D17-855F-B72FABA275E1}" name="Tareas" dataDxfId="688"/>
+    <tableColumn id="4" xr3:uid="{93A48342-846D-4345-B86E-84B03B9F5BE6}" name="Fecha de Entrega" dataDxfId="687"/>
+    <tableColumn id="5" xr3:uid="{A3806AAD-69B1-4B13-B2A6-2DE84CEE378A}" name="Anuncio" dataDxfId="686"/>
+    <tableColumn id="6" xr3:uid="{4DCE34DE-3E87-4BA4-9215-DC8689B0FB1F}" name="Mensaje" dataDxfId="685"/>
+    <tableColumn id="7" xr3:uid="{0F562F09-3842-4B56-A51E-DF3582B3119D}" name="Nota" dataDxfId="684"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{CBAFAA1F-486A-4F41-BFB3-2C37DBD3C8ED}" name="Tabla32" displayName="Tabla32" ref="B4:J7" totalsRowShown="0" headerRowDxfId="494" dataDxfId="493">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{CBAFAA1F-486A-4F41-BFB3-2C37DBD3C8ED}" name="Tabla32" displayName="Tabla32" ref="B4:J7" totalsRowShown="0" headerRowDxfId="501" dataDxfId="500">
   <autoFilter ref="B4:J7" xr:uid="{CBAFAA1F-486A-4F41-BFB3-2C37DBD3C8ED}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{85993DBD-620A-4565-BD7D-E67C38147719}" name="N.O Documento" dataDxfId="492"/>
-    <tableColumn id="2" xr3:uid="{2D813F1B-C294-48E8-9BA3-F55A13136210}" name="ID Documento" dataDxfId="491"/>
-    <tableColumn id="6" xr3:uid="{5DCA58FA-F5E0-4F7D-A728-DF8157504CFC}" name="Primer Nombre" dataDxfId="490"/>
-    <tableColumn id="7" xr3:uid="{81DBB017-5421-4C58-850E-8BBE4954F2F0}" name="Segundo Nombre" dataDxfId="489"/>
-    <tableColumn id="8" xr3:uid="{5B4E747C-2B7A-44F5-A5C0-91BE96C5BD39}" name="Primer Apellido" dataDxfId="488"/>
-    <tableColumn id="9" xr3:uid="{9B409E0A-541F-4FE3-A458-5C4DD925C532}" name="Segundo Apellido" dataDxfId="487"/>
-    <tableColumn id="4" xr3:uid="{7598CD6D-4377-4085-A8CE-124BC518E07C}" name="Correo 1" dataDxfId="486" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="3" xr3:uid="{B2E71AA3-EB87-4255-9646-DA8A21A8D891}" name="Contraseña" dataDxfId="485" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="10" xr3:uid="{38DA9B10-89CA-4796-9B9C-A4BA771580C6}" name="ID Rol" dataDxfId="484"/>
+    <tableColumn id="1" xr3:uid="{85993DBD-620A-4565-BD7D-E67C38147719}" name="N.O Documento" dataDxfId="499"/>
+    <tableColumn id="2" xr3:uid="{2D813F1B-C294-48E8-9BA3-F55A13136210}" name="ID Documento" dataDxfId="498"/>
+    <tableColumn id="6" xr3:uid="{5DCA58FA-F5E0-4F7D-A728-DF8157504CFC}" name="Primer Nombre" dataDxfId="497"/>
+    <tableColumn id="7" xr3:uid="{81DBB017-5421-4C58-850E-8BBE4954F2F0}" name="Segundo Nombre" dataDxfId="496"/>
+    <tableColumn id="8" xr3:uid="{5B4E747C-2B7A-44F5-A5C0-91BE96C5BD39}" name="Primer Apellido" dataDxfId="495"/>
+    <tableColumn id="9" xr3:uid="{9B409E0A-541F-4FE3-A458-5C4DD925C532}" name="Segundo Apellido" dataDxfId="494"/>
+    <tableColumn id="4" xr3:uid="{7598CD6D-4377-4085-A8CE-124BC518E07C}" name="Correo 1" dataDxfId="493" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="3" xr3:uid="{B2E71AA3-EB87-4255-9646-DA8A21A8D891}" name="Contraseña" dataDxfId="492" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="10" xr3:uid="{38DA9B10-89CA-4796-9B9C-A4BA771580C6}" name="ID Rol" dataDxfId="491"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{52DBBC11-DB63-4463-9018-9DFE38D063A5}" name="Tabla36" displayName="Tabla36" ref="B11:H14" totalsRowShown="0" headerRowDxfId="483" dataDxfId="481" headerRowBorderDxfId="482" tableBorderDxfId="480" totalsRowBorderDxfId="479">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{52DBBC11-DB63-4463-9018-9DFE38D063A5}" name="Tabla36" displayName="Tabla36" ref="B11:H14" totalsRowShown="0" headerRowDxfId="490" dataDxfId="488" headerRowBorderDxfId="489" tableBorderDxfId="487" totalsRowBorderDxfId="486">
   <autoFilter ref="B11:H14" xr:uid="{52DBBC11-DB63-4463-9018-9DFE38D063A5}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{28F25BAC-F99B-410F-88E4-0D0C698F85A9}" name="Informacion" dataDxfId="478"/>
-    <tableColumn id="5" xr3:uid="{1DF039EF-E304-40DE-B269-98CDAA18D624}" name="Correo 2" dataDxfId="477" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="6" xr3:uid="{E5ACB107-87D9-44ED-8344-CD8F804A52A2}" name="Contacto 1" dataDxfId="476"/>
-    <tableColumn id="7" xr3:uid="{201BDBA3-3ACB-4F10-93FC-2186EFD31FDA}" name="Contacto 2" dataDxfId="475"/>
-    <tableColumn id="9" xr3:uid="{743AAB21-3CCC-41BB-BF36-5E357C772CF3}" name="Fecha Nacimiento" dataDxfId="474"/>
-    <tableColumn id="10" xr3:uid="{17711778-5681-41B5-931B-87FFE721FE52}" name="Foto" dataDxfId="473"/>
-    <tableColumn id="2" xr3:uid="{7362A686-7195-4972-8A5F-2882DAA76512}" name="N.O Documento" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{28F25BAC-F99B-410F-88E4-0D0C698F85A9}" name="Informacion" dataDxfId="485"/>
+    <tableColumn id="5" xr3:uid="{1DF039EF-E304-40DE-B269-98CDAA18D624}" name="Correo 2" dataDxfId="484" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="6" xr3:uid="{E5ACB107-87D9-44ED-8344-CD8F804A52A2}" name="Contacto 1" dataDxfId="483"/>
+    <tableColumn id="7" xr3:uid="{201BDBA3-3ACB-4F10-93FC-2186EFD31FDA}" name="Contacto 2" dataDxfId="482"/>
+    <tableColumn id="9" xr3:uid="{743AAB21-3CCC-41BB-BF36-5E357C772CF3}" name="Fecha Nacimiento" dataDxfId="481"/>
+    <tableColumn id="10" xr3:uid="{17711778-5681-41B5-931B-87FFE721FE52}" name="Foto" dataDxfId="480"/>
+    <tableColumn id="2" xr3:uid="{7362A686-7195-4972-8A5F-2882DAA76512}" name="N.O Documento" dataDxfId="479"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{8EA7739E-5C69-4F63-8F5F-90ECC89721C1}" name="Tabla37" displayName="Tabla37" ref="J11:K14" totalsRowShown="0" headerRowDxfId="472" dataDxfId="470" headerRowBorderDxfId="471" tableBorderDxfId="469" totalsRowBorderDxfId="468">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{8EA7739E-5C69-4F63-8F5F-90ECC89721C1}" name="Tabla37" displayName="Tabla37" ref="J11:K14" totalsRowShown="0" headerRowDxfId="478" dataDxfId="476" headerRowBorderDxfId="477" tableBorderDxfId="475" totalsRowBorderDxfId="474">
   <autoFilter ref="J11:K14" xr:uid="{8EA7739E-5C69-4F63-8F5F-90ECC89721C1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E84CD73D-28D2-4690-AC8C-8DA131900484}" name="N.O Documento" dataDxfId="467"/>
-    <tableColumn id="2" xr3:uid="{935E8B09-2D0A-4976-B6D7-0565E499F9AE}" name="Curso" dataDxfId="466"/>
+    <tableColumn id="1" xr3:uid="{E84CD73D-28D2-4690-AC8C-8DA131900484}" name="N.O Documento" dataDxfId="473"/>
+    <tableColumn id="2" xr3:uid="{935E8B09-2D0A-4976-B6D7-0565E499F9AE}" name="Curso" dataDxfId="472"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{01EF36DC-E719-43B4-952F-EF102A871AAB}" name="Tabla2941" displayName="Tabla2941" ref="H18:L21" totalsRowShown="0" headerRowDxfId="465" dataDxfId="463" headerRowBorderDxfId="464" tableBorderDxfId="462" totalsRowBorderDxfId="461">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="40" xr:uid="{01EF36DC-E719-43B4-952F-EF102A871AAB}" name="Tabla2941" displayName="Tabla2941" ref="H18:L21" totalsRowShown="0" headerRowDxfId="471" dataDxfId="469" headerRowBorderDxfId="470" tableBorderDxfId="468" totalsRowBorderDxfId="467">
   <autoFilter ref="H18:L21" xr:uid="{01EF36DC-E719-43B4-952F-EF102A871AAB}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{107A85BB-4EF9-406C-B8E8-97D4ECDD5BF1}" name="ID Curso" dataDxfId="460"/>
-    <tableColumn id="2" xr3:uid="{A9ADAF75-EE40-41BC-A3C7-427D1398596D}" name="Curso" dataDxfId="459"/>
-    <tableColumn id="3" xr3:uid="{4BF41CD4-EF96-4668-BF94-2517A1ABDD0B}" name="Director" dataDxfId="458"/>
-    <tableColumn id="4" xr3:uid="{5EEA3EDC-5925-4956-B355-A619B05A3A32}" name="ID Jornada" dataDxfId="457"/>
-    <tableColumn id="5" xr3:uid="{FCEBA2AC-3519-4C34-9506-07A4C6B1278E}" name="Grado" dataDxfId="456"/>
+    <tableColumn id="1" xr3:uid="{107A85BB-4EF9-406C-B8E8-97D4ECDD5BF1}" name="ID Curso" dataDxfId="466"/>
+    <tableColumn id="2" xr3:uid="{A9ADAF75-EE40-41BC-A3C7-427D1398596D}" name="Curso" dataDxfId="465"/>
+    <tableColumn id="3" xr3:uid="{4BF41CD4-EF96-4668-BF94-2517A1ABDD0B}" name="Director" dataDxfId="464"/>
+    <tableColumn id="4" xr3:uid="{5EEA3EDC-5925-4956-B355-A619B05A3A32}" name="ID Jornada" dataDxfId="463"/>
+    <tableColumn id="5" xr3:uid="{FCEBA2AC-3519-4C34-9506-07A4C6B1278E}" name="Grado" dataDxfId="462"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{BE1D2972-DF9F-4A7D-86AA-7EB121605107}" name="Tabla344043" displayName="Tabla344043" ref="B18:C22" totalsRowShown="0" headerRowDxfId="455" dataDxfId="453" headerRowBorderDxfId="454" tableBorderDxfId="452" totalsRowBorderDxfId="451">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{BE1D2972-DF9F-4A7D-86AA-7EB121605107}" name="Tabla344043" displayName="Tabla344043" ref="B18:C22" totalsRowShown="0" headerRowDxfId="461" dataDxfId="459" headerRowBorderDxfId="460" tableBorderDxfId="458" totalsRowBorderDxfId="457">
   <autoFilter ref="B18:C22" xr:uid="{BE1D2972-DF9F-4A7D-86AA-7EB121605107}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8862089D-B2F4-4827-8295-A726A47F02F9}" name="ID Rol" dataDxfId="450"/>
-    <tableColumn id="2" xr3:uid="{0B2EA771-08A1-4240-BCB7-9533F0FC91A5}" name="Rol" dataDxfId="449"/>
+    <tableColumn id="1" xr3:uid="{8862089D-B2F4-4827-8295-A726A47F02F9}" name="ID Rol" dataDxfId="456"/>
+    <tableColumn id="2" xr3:uid="{0B2EA771-08A1-4240-BCB7-9533F0FC91A5}" name="Rol" dataDxfId="455"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{9D1035E7-0BEA-4FE4-841D-3F72DEB282A7}" name="Tabla27394244" displayName="Tabla27394244" ref="E18:F21" totalsRowShown="0" headerRowDxfId="448" dataDxfId="446" headerRowBorderDxfId="447" tableBorderDxfId="445" totalsRowBorderDxfId="444">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{9D1035E7-0BEA-4FE4-841D-3F72DEB282A7}" name="Tabla27394244" displayName="Tabla27394244" ref="E18:F21" totalsRowShown="0" headerRowDxfId="454" dataDxfId="452" headerRowBorderDxfId="453" tableBorderDxfId="451" totalsRowBorderDxfId="450">
   <autoFilter ref="E18:F21" xr:uid="{9D1035E7-0BEA-4FE4-841D-3F72DEB282A7}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{006AAF67-E5E0-4672-83BF-AA74259BD10E}" name="ID Documento" dataDxfId="443"/>
-    <tableColumn id="2" xr3:uid="{6177E073-A1E8-4E37-858A-97D4A8B54C5D}" name="Tipo Documento" dataDxfId="442"/>
+    <tableColumn id="1" xr3:uid="{006AAF67-E5E0-4672-83BF-AA74259BD10E}" name="ID Documento" dataDxfId="449"/>
+    <tableColumn id="2" xr3:uid="{6177E073-A1E8-4E37-858A-97D4A8B54C5D}" name="Tipo Documento" dataDxfId="448"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="47" xr:uid="{F29226EB-4B14-4152-9494-29F3A61B3F93}" name="Tabla47" displayName="Tabla47" ref="B26:E29" totalsRowShown="0" headerRowDxfId="441" dataDxfId="439" headerRowBorderDxfId="440" tableBorderDxfId="438" totalsRowBorderDxfId="437">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="47" xr:uid="{F29226EB-4B14-4152-9494-29F3A61B3F93}" name="Tabla47" displayName="Tabla47" ref="B26:E29" totalsRowShown="0" headerRowDxfId="447" dataDxfId="445" headerRowBorderDxfId="446" tableBorderDxfId="444" totalsRowBorderDxfId="443">
   <autoFilter ref="B26:E29" xr:uid="{F29226EB-4B14-4152-9494-29F3A61B3F93}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E758452A-1245-4BAB-9A71-26863B3627AE}" name="ID Horario" dataDxfId="436"/>
-    <tableColumn id="2" xr3:uid="{BD8799E3-527E-4EB9-9E02-5AB3B8165982}" name="Titulo Horario" dataDxfId="435"/>
-    <tableColumn id="3" xr3:uid="{F216016D-7C32-4295-BDB4-628A01486B4E}" name="Imagen Horario" dataDxfId="434"/>
-    <tableColumn id="4" xr3:uid="{05A1A193-5723-4D75-8915-168ACF286335}" name="Descripcion" dataDxfId="433"/>
+    <tableColumn id="1" xr3:uid="{E758452A-1245-4BAB-9A71-26863B3627AE}" name="ID Horario" dataDxfId="442"/>
+    <tableColumn id="2" xr3:uid="{BD8799E3-527E-4EB9-9E02-5AB3B8165982}" name="Titulo Horario" dataDxfId="441"/>
+    <tableColumn id="3" xr3:uid="{F216016D-7C32-4295-BDB4-628A01486B4E}" name="Imagen Horario" dataDxfId="440"/>
+    <tableColumn id="4" xr3:uid="{05A1A193-5723-4D75-8915-168ACF286335}" name="Descripcion" dataDxfId="439"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{96ACAA0C-267E-46C1-A7F5-B05F0E534C90}" name="Tabla38" displayName="Tabla38" ref="H26:I29" totalsRowShown="0" headerRowDxfId="432" dataDxfId="430" headerRowBorderDxfId="431" tableBorderDxfId="429" totalsRowBorderDxfId="428">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{96ACAA0C-267E-46C1-A7F5-B05F0E534C90}" name="Tabla38" displayName="Tabla38" ref="H26:I29" totalsRowShown="0" headerRowDxfId="438" dataDxfId="436" headerRowBorderDxfId="437" tableBorderDxfId="435" totalsRowBorderDxfId="434">
   <autoFilter ref="H26:I29" xr:uid="{96ACAA0C-267E-46C1-A7F5-B05F0E534C90}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{4288E401-D5E9-4A8D-B279-FB90114E33F3}" name="Curso" dataDxfId="427"/>
-    <tableColumn id="3" xr3:uid="{DA8A9AF6-F7E8-413B-B174-FCF874CF1F55}" name="Usuario" dataDxfId="426"/>
+    <tableColumn id="1" xr3:uid="{4288E401-D5E9-4A8D-B279-FB90114E33F3}" name="Curso" dataDxfId="433"/>
+    <tableColumn id="3" xr3:uid="{DA8A9AF6-F7E8-413B-B174-FCF874CF1F55}" name="Usuario" dataDxfId="432"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{7CDC0332-414C-4B90-A77F-914EF3A7199B}" name="Tabla39" displayName="Tabla39" ref="G26:G29" totalsRowShown="0" headerRowDxfId="425" dataDxfId="424">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{7CDC0332-414C-4B90-A77F-914EF3A7199B}" name="Tabla39" displayName="Tabla39" ref="G26:G29" totalsRowShown="0" headerRowDxfId="431" dataDxfId="430">
   <autoFilter ref="G26:G29" xr:uid="{7CDC0332-414C-4B90-A77F-914EF3A7199B}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{5F58DA05-DC65-4BD4-B69C-0FA6016CB2E4}" name="ID Horario" dataDxfId="423"/>
+    <tableColumn id="1" xr3:uid="{5F58DA05-DC65-4BD4-B69C-0FA6016CB2E4}" name="ID Horario" dataDxfId="429"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{7D927831-4F28-4765-939A-B20011C75F40}" name="Tabla41" displayName="Tabla41" ref="B41:G44" totalsRowShown="0" headerRowDxfId="422" dataDxfId="420" headerRowBorderDxfId="421">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{7D927831-4F28-4765-939A-B20011C75F40}" name="Tabla41" displayName="Tabla41" ref="B41:G44" totalsRowShown="0" headerRowDxfId="428" dataDxfId="426" headerRowBorderDxfId="427">
   <autoFilter ref="B41:G44" xr:uid="{7D927831-4F28-4765-939A-B20011C75F40}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{81FF2BFD-60E4-4792-B033-DD35AFB2B60E}" name="ID Anuncios" dataDxfId="419"/>
-    <tableColumn id="2" xr3:uid="{33E97C1B-09C6-40A0-B9D4-2494DE604772}" name="Titulo" dataDxfId="418"/>
-    <tableColumn id="3" xr3:uid="{6B540942-7D0B-499E-ABB6-27C1E28D881A}" name="Descripcion" dataDxfId="417"/>
-    <tableColumn id="4" xr3:uid="{C712F0DD-4F53-4BD0-B969-E5CEE16D3EBA}" name="Archivo Anuncio" dataDxfId="416"/>
-    <tableColumn id="5" xr3:uid="{44B9ABA4-0CCB-4047-A6D5-1B3C29E6AE6B}" name="Fecha" dataDxfId="415"/>
-    <tableColumn id="6" xr3:uid="{6C6D5FFC-4252-4F74-8616-0545F26D8849}" name="ID Aulas" dataDxfId="414"/>
+    <tableColumn id="1" xr3:uid="{81FF2BFD-60E4-4792-B033-DD35AFB2B60E}" name="ID Anuncios" dataDxfId="425"/>
+    <tableColumn id="2" xr3:uid="{33E97C1B-09C6-40A0-B9D4-2494DE604772}" name="Titulo" dataDxfId="424"/>
+    <tableColumn id="3" xr3:uid="{6B540942-7D0B-499E-ABB6-27C1E28D881A}" name="Descripcion" dataDxfId="423"/>
+    <tableColumn id="4" xr3:uid="{C712F0DD-4F53-4BD0-B969-E5CEE16D3EBA}" name="Archivo Anuncio" dataDxfId="422"/>
+    <tableColumn id="5" xr3:uid="{44B9ABA4-0CCB-4047-A6D5-1B3C29E6AE6B}" name="Fecha" dataDxfId="421"/>
+    <tableColumn id="6" xr3:uid="{6C6D5FFC-4252-4F74-8616-0545F26D8849}" name="ID Aulas" dataDxfId="420"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{5148F0FB-EFD1-4E5C-A565-3EDCC58C3E48}" name="Tabla18" displayName="Tabla18" ref="B17:E20" totalsRowShown="0" headerRowDxfId="676" dataDxfId="675">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{5148F0FB-EFD1-4E5C-A565-3EDCC58C3E48}" name="Tabla18" displayName="Tabla18" ref="B17:E20" totalsRowShown="0" headerRowDxfId="683" dataDxfId="682">
   <autoFilter ref="B17:E20" xr:uid="{5148F0FB-EFD1-4E5C-A565-3EDCC58C3E48}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{93F2F6E9-ABE3-417D-B82F-96A4C03A3AE3}" name="ID Planilla" dataDxfId="674"/>
-    <tableColumn id="2" xr3:uid="{05C116D7-FDDD-4971-9CC2-02DB3AF03D6B}" name="Nombre" dataDxfId="673"/>
-    <tableColumn id="3" xr3:uid="{768CA7BA-2998-4AD2-A7E2-4596828020DB}" name="ID Boletin" dataDxfId="672"/>
-    <tableColumn id="4" xr3:uid="{E080B043-AF0B-4340-9B9F-4CB5D02C6197}" name="Caracteristicas Boletin" dataDxfId="671"/>
+    <tableColumn id="1" xr3:uid="{93F2F6E9-ABE3-417D-B82F-96A4C03A3AE3}" name="ID Planilla" dataDxfId="681"/>
+    <tableColumn id="2" xr3:uid="{05C116D7-FDDD-4971-9CC2-02DB3AF03D6B}" name="Nombre" dataDxfId="680"/>
+    <tableColumn id="3" xr3:uid="{768CA7BA-2998-4AD2-A7E2-4596828020DB}" name="ID Boletin" dataDxfId="679"/>
+    <tableColumn id="4" xr3:uid="{E080B043-AF0B-4340-9B9F-4CB5D02C6197}" name="Caracteristicas Boletin" dataDxfId="678"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{7A26F7AA-DEB9-4AF4-A45D-A0052B805D5E}" name="Tabla50" displayName="Tabla50" ref="H34:J37" totalsRowShown="0" headerRowDxfId="413" dataDxfId="411" headerRowBorderDxfId="412" tableBorderDxfId="410" totalsRowBorderDxfId="409">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="50" xr:uid="{7A26F7AA-DEB9-4AF4-A45D-A0052B805D5E}" name="Tabla50" displayName="Tabla50" ref="H34:J37" totalsRowShown="0" headerRowDxfId="419" dataDxfId="417" headerRowBorderDxfId="418" tableBorderDxfId="416" totalsRowBorderDxfId="415">
   <autoFilter ref="H34:J37" xr:uid="{7A26F7AA-DEB9-4AF4-A45D-A0052B805D5E}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{824306FD-8689-401A-A88A-0C9CE74A2A2F}" name="ID Aula" dataDxfId="408"/>
-    <tableColumn id="2" xr3:uid="{1343048F-A584-4DA0-91A9-3A6D50B475E8}" name="ID Anuncios" dataDxfId="407"/>
-    <tableColumn id="3" xr3:uid="{24530E69-4691-4D5A-9DCE-AC14830B98FE}" name="ID Trabajos" dataDxfId="406"/>
+    <tableColumn id="1" xr3:uid="{824306FD-8689-401A-A88A-0C9CE74A2A2F}" name="ID Aula" dataDxfId="414"/>
+    <tableColumn id="2" xr3:uid="{1343048F-A584-4DA0-91A9-3A6D50B475E8}" name="ID Anuncios" dataDxfId="413"/>
+    <tableColumn id="3" xr3:uid="{24530E69-4691-4D5A-9DCE-AC14830B98FE}" name="ID Trabajos" dataDxfId="412"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table31.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="51" xr:uid="{AF0A0DDA-E267-485C-B72C-28015E8B2F83}" name="Tabla51" displayName="Tabla51" ref="I41:O44" totalsRowShown="0" headerRowDxfId="405" dataDxfId="403" headerRowBorderDxfId="404">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="51" xr:uid="{AF0A0DDA-E267-485C-B72C-28015E8B2F83}" name="Tabla51" displayName="Tabla51" ref="I41:O44" totalsRowShown="0" headerRowDxfId="411" dataDxfId="409" headerRowBorderDxfId="410">
   <autoFilter ref="I41:O44" xr:uid="{AF0A0DDA-E267-485C-B72C-28015E8B2F83}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{51341323-19CF-459D-9282-7DC703929F64}" name="ID Trabajos" dataDxfId="402"/>
-    <tableColumn id="2" xr3:uid="{599BC747-A3F1-4636-B4D5-713981D2FE1C}" name="Tema" dataDxfId="401"/>
-    <tableColumn id="3" xr3:uid="{EEEE6687-CF5B-40FB-8FA1-F8A851306587}" name="Titulo Trabajo" dataDxfId="400"/>
-    <tableColumn id="4" xr3:uid="{BE965E1C-281D-46C9-9FF0-5F16CA434DB0}" name="Descripcion" dataDxfId="399"/>
-    <tableColumn id="5" xr3:uid="{0A9CD567-C721-4284-ACF8-4F9D4A5380C1}" name="Fecha Entrega" dataDxfId="398"/>
-    <tableColumn id="6" xr3:uid="{0B1489B6-9829-4EF6-9086-2A18266B26F6}" name="Archivo" dataDxfId="397"/>
-    <tableColumn id="8" xr3:uid="{AE709390-DA2D-4E48-9E20-B158F621A506}" name="ID Aulas" dataDxfId="396"/>
+    <tableColumn id="1" xr3:uid="{51341323-19CF-459D-9282-7DC703929F64}" name="ID Trabajos" dataDxfId="408"/>
+    <tableColumn id="2" xr3:uid="{599BC747-A3F1-4636-B4D5-713981D2FE1C}" name="Tema" dataDxfId="407"/>
+    <tableColumn id="3" xr3:uid="{EEEE6687-CF5B-40FB-8FA1-F8A851306587}" name="Titulo Trabajo" dataDxfId="406"/>
+    <tableColumn id="4" xr3:uid="{BE965E1C-281D-46C9-9FF0-5F16CA434DB0}" name="Descripcion" dataDxfId="405"/>
+    <tableColumn id="5" xr3:uid="{0A9CD567-C721-4284-ACF8-4F9D4A5380C1}" name="Fecha Entrega" dataDxfId="404"/>
+    <tableColumn id="6" xr3:uid="{0B1489B6-9829-4EF6-9086-2A18266B26F6}" name="Archivo" dataDxfId="403"/>
+    <tableColumn id="8" xr3:uid="{AE709390-DA2D-4E48-9E20-B158F621A506}" name="ID Aulas" dataDxfId="402"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="53" xr:uid="{C189766A-FD92-4753-9F85-43E842E7F1F4}" name="Tabla53" displayName="Tabla53" ref="Q41:T44" totalsRowShown="0" headerRowDxfId="395" dataDxfId="393" headerRowBorderDxfId="394" tableBorderDxfId="392" totalsRowBorderDxfId="391">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="53" xr:uid="{C189766A-FD92-4753-9F85-43E842E7F1F4}" name="Tabla53" displayName="Tabla53" ref="Q41:T44" totalsRowShown="0" headerRowDxfId="401" dataDxfId="399" headerRowBorderDxfId="400" tableBorderDxfId="398" totalsRowBorderDxfId="397">
   <autoFilter ref="Q41:T44" xr:uid="{C189766A-FD92-4753-9F85-43E842E7F1F4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D1DBA655-232E-4F8A-9C7B-27B0572B485B}" name="ID Calificacion" dataDxfId="390"/>
-    <tableColumn id="2" xr3:uid="{C5F4B636-DD50-48C4-B090-FCBB54972E0F}" name="ID Alumno" dataDxfId="389"/>
-    <tableColumn id="3" xr3:uid="{212EC26D-41E6-4C37-9111-B80A66DF8823}" name="ID Trabajos" dataDxfId="388"/>
-    <tableColumn id="4" xr3:uid="{A6857211-9B8C-46F1-AD79-977FD091B8C7}" name="Nota" dataDxfId="387"/>
+    <tableColumn id="1" xr3:uid="{D1DBA655-232E-4F8A-9C7B-27B0572B485B}" name="ID Calificacion" dataDxfId="396"/>
+    <tableColumn id="2" xr3:uid="{C5F4B636-DD50-48C4-B090-FCBB54972E0F}" name="ID Alumno" dataDxfId="395"/>
+    <tableColumn id="3" xr3:uid="{212EC26D-41E6-4C37-9111-B80A66DF8823}" name="ID Trabajos" dataDxfId="394"/>
+    <tableColumn id="4" xr3:uid="{A6857211-9B8C-46F1-AD79-977FD091B8C7}" name="Nota" dataDxfId="393"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{EACF9940-7A1F-404C-9E9E-C140900CAF65}" name="Tabla2455" displayName="Tabla2455" ref="B48:F51" totalsRowShown="0" headerRowDxfId="386" dataDxfId="384" headerRowBorderDxfId="385" tableBorderDxfId="383" totalsRowBorderDxfId="382">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="54" xr:uid="{EACF9940-7A1F-404C-9E9E-C140900CAF65}" name="Tabla2455" displayName="Tabla2455" ref="B48:F51" totalsRowShown="0" headerRowDxfId="392" dataDxfId="390" headerRowBorderDxfId="391" tableBorderDxfId="389" totalsRowBorderDxfId="388">
   <autoFilter ref="B48:F51" xr:uid="{EACF9940-7A1F-404C-9E9E-C140900CAF65}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{174C31C9-B79E-403D-92E1-86032A79DCEA}" name="ID Notas" dataDxfId="381"/>
-    <tableColumn id="2" xr3:uid="{B769A7DC-C0B7-45ED-BE5D-CA07A72D8115}" name="ID Ususario" dataDxfId="380"/>
-    <tableColumn id="4" xr3:uid="{D2CBDFB8-C76B-45EC-A775-B4D8D8B19699}" name="ID Curso" dataDxfId="379"/>
-    <tableColumn id="5" xr3:uid="{CC0D41C6-0EAA-43C2-86DF-9E159A7864E8}" name="ID Materia " dataDxfId="378"/>
-    <tableColumn id="6" xr3:uid="{241D12A7-FFB1-4264-8F00-5E10751C6AE0}" name="Nota Final " dataDxfId="377"/>
+    <tableColumn id="1" xr3:uid="{174C31C9-B79E-403D-92E1-86032A79DCEA}" name="ID Notas" dataDxfId="387"/>
+    <tableColumn id="2" xr3:uid="{B769A7DC-C0B7-45ED-BE5D-CA07A72D8115}" name="ID Ususario" dataDxfId="386"/>
+    <tableColumn id="4" xr3:uid="{D2CBDFB8-C76B-45EC-A775-B4D8D8B19699}" name="ID Curso" dataDxfId="385"/>
+    <tableColumn id="5" xr3:uid="{CC0D41C6-0EAA-43C2-86DF-9E159A7864E8}" name="ID Materia " dataDxfId="384"/>
+    <tableColumn id="6" xr3:uid="{241D12A7-FFB1-4264-8F00-5E10751C6AE0}" name="Nota Final " dataDxfId="383"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="55" xr:uid="{8F2EB5F0-7076-459A-969B-63D255D67C74}" name="Tabla4456" displayName="Tabla4456" ref="M11:N14" totalsRowShown="0" headerRowDxfId="376" dataDxfId="374" headerRowBorderDxfId="375" tableBorderDxfId="373" totalsRowBorderDxfId="372">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="55" xr:uid="{8F2EB5F0-7076-459A-969B-63D255D67C74}" name="Tabla4456" displayName="Tabla4456" ref="M11:N14" totalsRowShown="0" headerRowDxfId="382" dataDxfId="380" headerRowBorderDxfId="381" tableBorderDxfId="379" totalsRowBorderDxfId="378">
   <autoFilter ref="M11:N14" xr:uid="{8F2EB5F0-7076-459A-969B-63D255D67C74}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3379AC82-CEF1-4B98-ACF4-1C0D4F8D4932}" name="ID Curso" dataDxfId="371"/>
-    <tableColumn id="2" xr3:uid="{30F45BBC-F494-4875-82AE-3D6464F038EF}" name="Miembros" dataDxfId="370"/>
+    <tableColumn id="1" xr3:uid="{3379AC82-CEF1-4B98-ACF4-1C0D4F8D4932}" name="ID Curso" dataDxfId="377"/>
+    <tableColumn id="2" xr3:uid="{30F45BBC-F494-4875-82AE-3D6464F038EF}" name="Miembros" dataDxfId="376"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{9E655B88-913D-4DF0-A55D-F23D4B21F096}" name="Tabla2357" displayName="Tabla2357" ref="B55:F58" totalsRowShown="0" headerRowDxfId="369" dataDxfId="367" headerRowBorderDxfId="368" tableBorderDxfId="366" totalsRowBorderDxfId="365">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="56" xr:uid="{9E655B88-913D-4DF0-A55D-F23D4B21F096}" name="Tabla2357" displayName="Tabla2357" ref="B55:F58" totalsRowShown="0" headerRowDxfId="375" dataDxfId="373" headerRowBorderDxfId="374" tableBorderDxfId="372" totalsRowBorderDxfId="371">
   <autoFilter ref="B55:F58" xr:uid="{9E655B88-913D-4DF0-A55D-F23D4B21F096}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4B83A15C-10E2-4B42-ADF0-6B4BD66D352F}" name="ID Planilla" dataDxfId="364"/>
-    <tableColumn id="2" xr3:uid="{34B3282F-3265-4983-9233-0E0EFD180F64}" name="Nombre Planilla" dataDxfId="363"/>
-    <tableColumn id="3" xr3:uid="{AB38E50F-DAF0-42B0-9189-6EA7E488444A}" name="ID Curso" dataDxfId="362"/>
-    <tableColumn id="5" xr3:uid="{CC9850FB-052E-4337-9423-0062D4C8E48A}" name="ID Periodo" dataDxfId="361"/>
-    <tableColumn id="6" xr3:uid="{DE9CA131-DA4E-4E3A-837A-56C2B3D20A41}" name="ID Nota Final" dataDxfId="360"/>
+    <tableColumn id="1" xr3:uid="{4B83A15C-10E2-4B42-ADF0-6B4BD66D352F}" name="ID Planilla" dataDxfId="370"/>
+    <tableColumn id="2" xr3:uid="{34B3282F-3265-4983-9233-0E0EFD180F64}" name="Nombre Planilla" dataDxfId="369"/>
+    <tableColumn id="3" xr3:uid="{AB38E50F-DAF0-42B0-9189-6EA7E488444A}" name="ID Curso" dataDxfId="368"/>
+    <tableColumn id="5" xr3:uid="{CC9850FB-052E-4337-9423-0062D4C8E48A}" name="ID Periodo" dataDxfId="367"/>
+    <tableColumn id="6" xr3:uid="{DE9CA131-DA4E-4E3A-837A-56C2B3D20A41}" name="ID Nota Final" dataDxfId="366"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{50A26314-7E24-4725-8821-4FD0E3C9DA69}" name="Tabla3159" displayName="Tabla3159" ref="H55:I59" totalsRowShown="0" headerRowDxfId="359" dataDxfId="357" headerRowBorderDxfId="358" tableBorderDxfId="356" totalsRowBorderDxfId="355">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="58" xr:uid="{50A26314-7E24-4725-8821-4FD0E3C9DA69}" name="Tabla3159" displayName="Tabla3159" ref="H55:I59" totalsRowShown="0" headerRowDxfId="365" dataDxfId="363" headerRowBorderDxfId="364" tableBorderDxfId="362" totalsRowBorderDxfId="361">
   <autoFilter ref="H55:I59" xr:uid="{50A26314-7E24-4725-8821-4FD0E3C9DA69}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F7C56F7E-D071-4A47-AEF6-91B7A62DE01C}" name="ID Perido" dataDxfId="354"/>
-    <tableColumn id="2" xr3:uid="{F67DDD2F-51B4-4C2F-B768-87F6AADC2129}" name="Periodo" dataDxfId="353"/>
+    <tableColumn id="1" xr3:uid="{F7C56F7E-D071-4A47-AEF6-91B7A62DE01C}" name="ID Perido" dataDxfId="360"/>
+    <tableColumn id="2" xr3:uid="{F67DDD2F-51B4-4C2F-B768-87F6AADC2129}" name="Periodo" dataDxfId="359"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{A38B8536-84C4-4EA7-BE2C-DD24D5F0069A}" name="Tabla59" displayName="Tabla59" ref="B62:G65" totalsRowShown="0" headerRowDxfId="352" dataDxfId="350" headerRowBorderDxfId="351" tableBorderDxfId="349" totalsRowBorderDxfId="348">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="59" xr:uid="{A38B8536-84C4-4EA7-BE2C-DD24D5F0069A}" name="Tabla59" displayName="Tabla59" ref="B62:G65" totalsRowShown="0" headerRowDxfId="358" dataDxfId="356" headerRowBorderDxfId="357" tableBorderDxfId="355" totalsRowBorderDxfId="354">
   <autoFilter ref="B62:G65" xr:uid="{A38B8536-84C4-4EA7-BE2C-DD24D5F0069A}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D2D62F8C-2B08-4E0A-8FF2-DBF26164BA78}" name="ID Boletin" dataDxfId="347"/>
-    <tableColumn id="2" xr3:uid="{6596522C-841F-47FC-AF39-3EF21C6F064D}" name="Nombre " dataDxfId="346"/>
-    <tableColumn id="3" xr3:uid="{C017E5F5-3FDC-44AA-96FB-DC85BC1F577F}" name="Institucion" dataDxfId="345"/>
-    <tableColumn id="4" xr3:uid="{B1C1D52C-F1A9-41C8-BED9-F8E99905550A}" name="Sede" dataDxfId="344"/>
-    <tableColumn id="5" xr3:uid="{4BBD0387-9487-459D-8306-29EF1FAFE118}" name="Año" dataDxfId="343"/>
-    <tableColumn id="6" xr3:uid="{DF2D5CF2-3686-4FAD-9C05-6BDFD9431428}" name="Resolucion" dataDxfId="342"/>
+    <tableColumn id="1" xr3:uid="{D2D62F8C-2B08-4E0A-8FF2-DBF26164BA78}" name="ID Boletin" dataDxfId="353"/>
+    <tableColumn id="2" xr3:uid="{6596522C-841F-47FC-AF39-3EF21C6F064D}" name="Nombre " dataDxfId="352"/>
+    <tableColumn id="3" xr3:uid="{C017E5F5-3FDC-44AA-96FB-DC85BC1F577F}" name="Institucion" dataDxfId="351"/>
+    <tableColumn id="4" xr3:uid="{B1C1D52C-F1A9-41C8-BED9-F8E99905550A}" name="Sede" dataDxfId="350"/>
+    <tableColumn id="5" xr3:uid="{4BBD0387-9487-459D-8306-29EF1FAFE118}" name="Año" dataDxfId="349"/>
+    <tableColumn id="6" xr3:uid="{DF2D5CF2-3686-4FAD-9C05-6BDFD9431428}" name="Resolucion" dataDxfId="348"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table38.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="61" xr:uid="{ABFED763-ED0F-4382-BFBF-1E5A1202FC42}" name="Tabla61" displayName="Tabla61" ref="M48:Q51" totalsRowShown="0" headerRowDxfId="341" dataDxfId="339" headerRowBorderDxfId="340" tableBorderDxfId="338" totalsRowBorderDxfId="337">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="61" xr:uid="{ABFED763-ED0F-4382-BFBF-1E5A1202FC42}" name="Tabla61" displayName="Tabla61" ref="M48:Q51" totalsRowShown="0" headerRowDxfId="347" dataDxfId="345" headerRowBorderDxfId="346" tableBorderDxfId="344" totalsRowBorderDxfId="343">
   <autoFilter ref="M48:Q51" xr:uid="{ABFED763-ED0F-4382-BFBF-1E5A1202FC42}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{3FDA7253-049E-405D-A9BB-000F2378AD97}" name="ID Calificacion" dataDxfId="336"/>
-    <tableColumn id="2" xr3:uid="{4A8802AF-254E-46CF-A563-23D73A6C358D}" name="Nota Final" dataDxfId="335"/>
-    <tableColumn id="3" xr3:uid="{35744070-E136-46C3-BB62-F3D946EC6B0A}" name="ID Logro" dataDxfId="334"/>
-    <tableColumn id="4" xr3:uid="{5C0BF754-50E8-454D-A74D-1A0F86412CCF}" name="Inasistencias" dataDxfId="333"/>
-    <tableColumn id="5" xr3:uid="{DCEF98E4-BFEA-451D-813D-DED1871A5F0D}" name="ID Materia" dataDxfId="332"/>
+    <tableColumn id="1" xr3:uid="{3FDA7253-049E-405D-A9BB-000F2378AD97}" name="ID Calificacion" dataDxfId="342"/>
+    <tableColumn id="2" xr3:uid="{4A8802AF-254E-46CF-A563-23D73A6C358D}" name="Nota Final" dataDxfId="341"/>
+    <tableColumn id="3" xr3:uid="{35744070-E136-46C3-BB62-F3D946EC6B0A}" name="ID Logro" dataDxfId="340"/>
+    <tableColumn id="4" xr3:uid="{5C0BF754-50E8-454D-A74D-1A0F86412CCF}" name="Inasistencias" dataDxfId="339"/>
+    <tableColumn id="5" xr3:uid="{DCEF98E4-BFEA-451D-813D-DED1871A5F0D}" name="ID Materia" dataDxfId="338"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table39.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="63" xr:uid="{46B2A6FC-D7DF-4EF2-A86B-2E7A8EF79342}" name="Tabla63" displayName="Tabla63" ref="S48:T51" totalsRowShown="0" headerRowDxfId="331" dataDxfId="329" headerRowBorderDxfId="330" tableBorderDxfId="328" totalsRowBorderDxfId="327">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="63" xr:uid="{46B2A6FC-D7DF-4EF2-A86B-2E7A8EF79342}" name="Tabla63" displayName="Tabla63" ref="S48:T51" totalsRowShown="0" headerRowDxfId="337" dataDxfId="335" headerRowBorderDxfId="336" tableBorderDxfId="334" totalsRowBorderDxfId="333">
   <autoFilter ref="S48:T51" xr:uid="{46B2A6FC-D7DF-4EF2-A86B-2E7A8EF79342}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5D263195-F69D-4193-9B40-C24A245933FC}" name="ID Logro2" dataDxfId="326"/>
-    <tableColumn id="2" xr3:uid="{85AEBD94-EF1E-4C99-833C-8C08D8BD4486}" name="Logro" dataDxfId="325"/>
+    <tableColumn id="1" xr3:uid="{5D263195-F69D-4193-9B40-C24A245933FC}" name="ID Logro2" dataDxfId="332"/>
+    <tableColumn id="2" xr3:uid="{85AEBD94-EF1E-4C99-833C-8C08D8BD4486}" name="Logro" dataDxfId="331"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{03C409CF-5B7A-4181-BBB6-C718A1105C65}" name="Tabla19" displayName="Tabla19" ref="B24:F27" totalsRowShown="0" headerRowDxfId="670" dataDxfId="668" headerRowBorderDxfId="669" tableBorderDxfId="667" totalsRowBorderDxfId="666">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{03C409CF-5B7A-4181-BBB6-C718A1105C65}" name="Tabla19" displayName="Tabla19" ref="B24:F27" totalsRowShown="0" headerRowDxfId="677" dataDxfId="675" headerRowBorderDxfId="676" tableBorderDxfId="674" totalsRowBorderDxfId="673">
   <autoFilter ref="B24:F27" xr:uid="{03C409CF-5B7A-4181-BBB6-C718A1105C65}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C00B1BF6-3FB6-41F4-8CF0-D701836ED230}" name="ID Noticias" dataDxfId="665"/>
-    <tableColumn id="2" xr3:uid="{EDDF096C-6E8F-414A-8861-5606C6A081FE}" name="Titulo" dataDxfId="664"/>
-    <tableColumn id="3" xr3:uid="{07363D8A-E737-4E51-954F-59C657E09E05}" name="Descripcion" dataDxfId="663"/>
-    <tableColumn id="4" xr3:uid="{84F20BDE-197E-45DC-988A-E332DA37B99F}" name="Fecha" dataDxfId="662"/>
-    <tableColumn id="5" xr3:uid="{8A4A3B42-92DA-4F1F-B1FB-20AFB21EE838}" name="Tipo" dataDxfId="661"/>
+    <tableColumn id="1" xr3:uid="{C00B1BF6-3FB6-41F4-8CF0-D701836ED230}" name="ID Noticias" dataDxfId="672"/>
+    <tableColumn id="2" xr3:uid="{EDDF096C-6E8F-414A-8861-5606C6A081FE}" name="Titulo" dataDxfId="671"/>
+    <tableColumn id="3" xr3:uid="{07363D8A-E737-4E51-954F-59C657E09E05}" name="Descripcion" dataDxfId="670"/>
+    <tableColumn id="4" xr3:uid="{84F20BDE-197E-45DC-988A-E332DA37B99F}" name="Fecha" dataDxfId="669"/>
+    <tableColumn id="5" xr3:uid="{8A4A3B42-92DA-4F1F-B1FB-20AFB21EE838}" name="Tipo" dataDxfId="668"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table40.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="64" xr:uid="{1FA7F686-7F62-4EA5-AA38-F770ED42D9A1}" name="Tabla3565" displayName="Tabla3565" ref="P11:Q14" totalsRowShown="0" headerRowDxfId="324" dataDxfId="322" headerRowBorderDxfId="323" tableBorderDxfId="321" totalsRowBorderDxfId="320">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="64" xr:uid="{1FA7F686-7F62-4EA5-AA38-F770ED42D9A1}" name="Tabla3565" displayName="Tabla3565" ref="P11:Q14" totalsRowShown="0" headerRowDxfId="330" dataDxfId="328" headerRowBorderDxfId="329" tableBorderDxfId="327" totalsRowBorderDxfId="326">
   <autoFilter ref="P11:Q14" xr:uid="{1FA7F686-7F62-4EA5-AA38-F770ED42D9A1}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A6E6275E-D6B6-4CAF-B826-D4F04E3591A2}" name="ID Materia" dataDxfId="319"/>
-    <tableColumn id="2" xr3:uid="{6A0C0DC0-12E5-4858-94F4-C52D7838EF9F}" name="Materia" dataDxfId="318"/>
+    <tableColumn id="1" xr3:uid="{A6E6275E-D6B6-4CAF-B826-D4F04E3591A2}" name="ID Materia" dataDxfId="325"/>
+    <tableColumn id="2" xr3:uid="{6A0C0DC0-12E5-4858-94F4-C52D7838EF9F}" name="Materia" dataDxfId="324"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table41.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="65" xr:uid="{25372C2B-0E59-41AA-8C04-0B582BE2C712}" name="Tabla192766" displayName="Tabla192766" ref="B69:I72" totalsRowShown="0" headerRowDxfId="317" dataDxfId="315" headerRowBorderDxfId="316" tableBorderDxfId="314" totalsRowBorderDxfId="313">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="65" xr:uid="{25372C2B-0E59-41AA-8C04-0B582BE2C712}" name="Tabla192766" displayName="Tabla192766" ref="B69:I72" totalsRowShown="0" headerRowDxfId="323" dataDxfId="321" headerRowBorderDxfId="322" tableBorderDxfId="320" totalsRowBorderDxfId="319">
   <autoFilter ref="B69:I72" xr:uid="{25372C2B-0E59-41AA-8C04-0B582BE2C712}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{7EFCD0F7-1C0E-4578-8BD4-50B06B6D0CF1}" name="ID Noticias" dataDxfId="312"/>
-    <tableColumn id="2" xr3:uid="{ED4B09B4-CBA7-4A80-A883-D38B0F20DC83}" name="Titulo" dataDxfId="311"/>
-    <tableColumn id="3" xr3:uid="{30082752-B245-47BD-8863-315EA427AB75}" name="Descripcion" dataDxfId="310"/>
-    <tableColumn id="4" xr3:uid="{41F7D74D-49F3-4D5B-A367-B9509776967D}" name="Fecha" dataDxfId="309"/>
-    <tableColumn id="5" xr3:uid="{982FD9DC-86ED-4004-9C0B-7EB8D6BAB314}" name="ID Tipo" dataDxfId="308"/>
-    <tableColumn id="6" xr3:uid="{8751FA79-9BC9-461D-8E70-71312929ABF9}" name="Imagen 1" dataDxfId="307"/>
-    <tableColumn id="7" xr3:uid="{695D1E19-05FC-478D-8A22-5DE3CA986464}" name="Imagen 2" dataDxfId="306"/>
-    <tableColumn id="8" xr3:uid="{6C160B98-DF54-41AE-99D3-703E00D119D5}" name="Imagen 3" dataDxfId="305"/>
+    <tableColumn id="1" xr3:uid="{7EFCD0F7-1C0E-4578-8BD4-50B06B6D0CF1}" name="ID Noticias" dataDxfId="318"/>
+    <tableColumn id="2" xr3:uid="{ED4B09B4-CBA7-4A80-A883-D38B0F20DC83}" name="Titulo" dataDxfId="317"/>
+    <tableColumn id="3" xr3:uid="{30082752-B245-47BD-8863-315EA427AB75}" name="Descripcion" dataDxfId="316"/>
+    <tableColumn id="4" xr3:uid="{41F7D74D-49F3-4D5B-A367-B9509776967D}" name="Fecha" dataDxfId="315"/>
+    <tableColumn id="5" xr3:uid="{982FD9DC-86ED-4004-9C0B-7EB8D6BAB314}" name="ID Tipo" dataDxfId="314"/>
+    <tableColumn id="6" xr3:uid="{8751FA79-9BC9-461D-8E70-71312929ABF9}" name="Imagen 1" dataDxfId="313"/>
+    <tableColumn id="7" xr3:uid="{695D1E19-05FC-478D-8A22-5DE3CA986464}" name="Imagen 2" dataDxfId="312"/>
+    <tableColumn id="8" xr3:uid="{6C160B98-DF54-41AE-99D3-703E00D119D5}" name="Imagen 3" dataDxfId="311"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table42.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="67" xr:uid="{73AFC823-90C9-493D-BC9A-8C9C560B8436}" name="Tabla3368" displayName="Tabla3368" ref="N69:O73" totalsRowShown="0" headerRowDxfId="304" dataDxfId="302" headerRowBorderDxfId="303" tableBorderDxfId="301" totalsRowBorderDxfId="300">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="67" xr:uid="{73AFC823-90C9-493D-BC9A-8C9C560B8436}" name="Tabla3368" displayName="Tabla3368" ref="N69:O73" totalsRowShown="0" headerRowDxfId="310" dataDxfId="308" headerRowBorderDxfId="309" tableBorderDxfId="307" totalsRowBorderDxfId="306">
   <autoFilter ref="N69:O73" xr:uid="{73AFC823-90C9-493D-BC9A-8C9C560B8436}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{5B9393E9-9710-4B48-92BD-6E395E7A1969}" name="ID Valoracion" dataDxfId="299"/>
-    <tableColumn id="2" xr3:uid="{66D432ED-8F07-4894-8A36-B9BF2EB4F065}" name="Valoracion" dataDxfId="298"/>
+    <tableColumn id="1" xr3:uid="{5B9393E9-9710-4B48-92BD-6E395E7A1969}" name="ID Valoracion" dataDxfId="305"/>
+    <tableColumn id="2" xr3:uid="{66D432ED-8F07-4894-8A36-B9BF2EB4F065}" name="Valoracion" dataDxfId="304"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table43.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="49" xr:uid="{06C7D3FA-3861-43D7-A2D9-F620E1B63B81}" name="Tabla30464550" displayName="Tabla30464550" ref="N18:O21" totalsRowShown="0" headerRowDxfId="297" dataDxfId="295" headerRowBorderDxfId="296" tableBorderDxfId="294" totalsRowBorderDxfId="293">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="49" xr:uid="{06C7D3FA-3861-43D7-A2D9-F620E1B63B81}" name="Tabla30464550" displayName="Tabla30464550" ref="N18:O21" totalsRowShown="0" headerRowDxfId="303" dataDxfId="301" headerRowBorderDxfId="302" tableBorderDxfId="300" totalsRowBorderDxfId="299">
   <autoFilter ref="N18:O21" xr:uid="{06C7D3FA-3861-43D7-A2D9-F620E1B63B81}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{37B1C790-8AE0-49CB-8C21-0A59ABDEECA2}" name="ID Grado" dataDxfId="292"/>
-    <tableColumn id="2" xr3:uid="{1AF14EBE-18EC-4F69-AA21-81B27596A00C}" name="Grado" dataDxfId="291"/>
+    <tableColumn id="1" xr3:uid="{37B1C790-8AE0-49CB-8C21-0A59ABDEECA2}" name="ID Grado" dataDxfId="298"/>
+    <tableColumn id="2" xr3:uid="{1AF14EBE-18EC-4F69-AA21-81B27596A00C}" name="Grado" dataDxfId="297"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table44.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{2B78B6C6-ED39-4307-881A-1F33A2E0C69E}" name="Tabla28474953" displayName="Tabla28474953" ref="Q18:R20" totalsRowShown="0" headerRowDxfId="290" dataDxfId="288" headerRowBorderDxfId="289" tableBorderDxfId="287" totalsRowBorderDxfId="286">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="52" xr:uid="{2B78B6C6-ED39-4307-881A-1F33A2E0C69E}" name="Tabla28474953" displayName="Tabla28474953" ref="Q18:R20" totalsRowShown="0" headerRowDxfId="296" dataDxfId="294" headerRowBorderDxfId="295" tableBorderDxfId="293" totalsRowBorderDxfId="292">
   <autoFilter ref="Q18:R20" xr:uid="{2B78B6C6-ED39-4307-881A-1F33A2E0C69E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{37B7A53A-E7F8-4D43-9BA8-E5E28252005F}" name="ID Jornada" dataDxfId="285"/>
-    <tableColumn id="2" xr3:uid="{D24C8425-76E5-4ADC-A626-39E189F6379C}" name="Jornada" dataDxfId="284"/>
+    <tableColumn id="1" xr3:uid="{37B7A53A-E7F8-4D43-9BA8-E5E28252005F}" name="ID Jornada" dataDxfId="291"/>
+    <tableColumn id="2" xr3:uid="{D24C8425-76E5-4ADC-A626-39E189F6379C}" name="Jornada" dataDxfId="290"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table45.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="79" xr:uid="{AA6F71D4-A815-45BC-AE6D-EB6B7C1BE5A7}" name="Tabla79" displayName="Tabla79" ref="I62:L65" totalsRowShown="0" headerRowDxfId="283" headerRowBorderDxfId="282" tableBorderDxfId="281" totalsRowBorderDxfId="280">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="79" xr:uid="{AA6F71D4-A815-45BC-AE6D-EB6B7C1BE5A7}" name="Tabla79" displayName="Tabla79" ref="I62:L65" totalsRowShown="0" headerRowDxfId="289" headerRowBorderDxfId="288" tableBorderDxfId="287" totalsRowBorderDxfId="286">
   <autoFilter ref="I62:L65" xr:uid="{AA6F71D4-A815-45BC-AE6D-EB6B7C1BE5A7}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{16190DC0-A2F5-4529-806C-4583DA4B068D}" name="ID Boletin" dataDxfId="279"/>
-    <tableColumn id="2" xr3:uid="{0FA533D4-CD6F-4518-8722-9FCE24F372CC}" name="Estudiante" dataDxfId="278"/>
-    <tableColumn id="3" xr3:uid="{55DA2D01-5777-4936-9244-546310FDAE40}" name="ID Perido" dataDxfId="277"/>
-    <tableColumn id="4" xr3:uid="{23A5BC91-F949-420B-8F0C-4F2FD5D6273B}" name="ID Boletin Detalles" dataDxfId="276"/>
+    <tableColumn id="1" xr3:uid="{16190DC0-A2F5-4529-806C-4583DA4B068D}" name="ID Boletin" dataDxfId="285"/>
+    <tableColumn id="2" xr3:uid="{0FA533D4-CD6F-4518-8722-9FCE24F372CC}" name="Estudiante" dataDxfId="284"/>
+    <tableColumn id="3" xr3:uid="{55DA2D01-5777-4936-9244-546310FDAE40}" name="ID Perido" dataDxfId="283"/>
+    <tableColumn id="4" xr3:uid="{23A5BC91-F949-420B-8F0C-4F2FD5D6273B}" name="ID Boletin Detalles" dataDxfId="282"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table46.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="80" xr:uid="{EBEB983E-49A0-4904-BD2C-E25EA34A5214}" name="Tabla607981" displayName="Tabla607981" ref="V62:Z65" totalsRowShown="0" headerRowDxfId="275" dataDxfId="273" headerRowBorderDxfId="274" tableBorderDxfId="272" totalsRowBorderDxfId="271">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="80" xr:uid="{EBEB983E-49A0-4904-BD2C-E25EA34A5214}" name="Tabla607981" displayName="Tabla607981" ref="V62:Z65" totalsRowShown="0" headerRowDxfId="281" dataDxfId="279" headerRowBorderDxfId="280" tableBorderDxfId="278" totalsRowBorderDxfId="277">
   <autoFilter ref="V62:Z65" xr:uid="{EBEB983E-49A0-4904-BD2C-E25EA34A5214}"/>
   <tableColumns count="5">
-    <tableColumn id="13" xr3:uid="{14ABB9C6-6967-45FD-8240-B6A794B592D3}" name="Fallas " dataDxfId="270"/>
-    <tableColumn id="14" xr3:uid="{851633F8-7176-4970-8E70-D36CD606EFFC}" name="Puesto" dataDxfId="269"/>
-    <tableColumn id="15" xr3:uid="{FD755439-3501-4C3A-8762-FC2E3A044A5A}" name="ID Valoracion" dataDxfId="268"/>
-    <tableColumn id="16" xr3:uid="{0B121205-705D-4E1A-8D63-CC3CDB1B19DF}" name="Comportamiento" dataDxfId="267"/>
-    <tableColumn id="17" xr3:uid="{B1D479EB-163F-4468-99CF-A4785F750CBC}" name="Observaciones" dataDxfId="266"/>
+    <tableColumn id="13" xr3:uid="{14ABB9C6-6967-45FD-8240-B6A794B592D3}" name="Fallas " dataDxfId="276"/>
+    <tableColumn id="14" xr3:uid="{851633F8-7176-4970-8E70-D36CD606EFFC}" name="Puesto" dataDxfId="275"/>
+    <tableColumn id="15" xr3:uid="{FD755439-3501-4C3A-8762-FC2E3A044A5A}" name="ID Valoracion" dataDxfId="274"/>
+    <tableColumn id="16" xr3:uid="{0B121205-705D-4E1A-8D63-CC3CDB1B19DF}" name="Comportamiento" dataDxfId="273"/>
+    <tableColumn id="17" xr3:uid="{B1D479EB-163F-4468-99CF-A4785F750CBC}" name="Observaciones" dataDxfId="272"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table47.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89039618-33D3-4F9C-B2E2-AE7BBF0D2689}" name="Tabla1" displayName="Tabla1" ref="K69:L72" totalsRowShown="0" headerRowDxfId="265" headerRowBorderDxfId="264" tableBorderDxfId="263" totalsRowBorderDxfId="262">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89039618-33D3-4F9C-B2E2-AE7BBF0D2689}" name="Tabla1" displayName="Tabla1" ref="K69:L72" totalsRowShown="0" headerRowDxfId="271" headerRowBorderDxfId="270" tableBorderDxfId="269" totalsRowBorderDxfId="268">
   <autoFilter ref="K69:L72" xr:uid="{89039618-33D3-4F9C-B2E2-AE7BBF0D2689}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{94C214A0-191A-44C5-81F0-903B3B54F608}" name="ID Tipo" dataDxfId="261"/>
-    <tableColumn id="2" xr3:uid="{72834F1F-D264-4ED5-AA7E-43250122B8A4}" name="Tipos" dataDxfId="260"/>
+    <tableColumn id="1" xr3:uid="{94C214A0-191A-44C5-81F0-903B3B54F608}" name="ID Tipo" dataDxfId="267"/>
+    <tableColumn id="2" xr3:uid="{72834F1F-D264-4ED5-AA7E-43250122B8A4}" name="Tipos" dataDxfId="266"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table48.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="57" xr:uid="{06EE946E-0446-4BD1-892A-BBC07F18241A}" name="Tabla3258" displayName="Tabla3258" ref="B3:J6" totalsRowShown="0" headerRowDxfId="259" dataDxfId="258">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="57" xr:uid="{06EE946E-0446-4BD1-892A-BBC07F18241A}" name="Tabla3258" displayName="Tabla3258" ref="B3:J6" totalsRowShown="0" headerRowDxfId="265" dataDxfId="264">
   <autoFilter ref="B3:J6" xr:uid="{06EE946E-0446-4BD1-892A-BBC07F18241A}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{851FE67B-C5F3-4094-A11C-923C88F6F300}" name="N.O Documento" dataDxfId="257"/>
-    <tableColumn id="2" xr3:uid="{2632ED65-1042-4D3A-ADC9-D4D0B903999F}" name="ID Documento" dataDxfId="256"/>
-    <tableColumn id="6" xr3:uid="{ABDF7375-83D9-47F3-8016-805F94AE16CC}" name="Primer Nombre" dataDxfId="255"/>
-    <tableColumn id="7" xr3:uid="{C91A11A7-C386-41E9-9560-C1514895842B}" name="Segundo Nombre" dataDxfId="254"/>
-    <tableColumn id="8" xr3:uid="{D75C02DF-B566-48D0-BCEF-1EEAF6C1DBA0}" name="Primer Apellido" dataDxfId="253"/>
-    <tableColumn id="4" xr3:uid="{38E42D0E-DFE7-454C-A189-559E10304022}" name="Segundo Apellido" dataDxfId="252"/>
-    <tableColumn id="9" xr3:uid="{01E3696D-3324-41C5-B5B9-D38D921838B9}" name="Correo 1" dataDxfId="251" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="5" xr3:uid="{6042456D-7E56-4678-804F-8C45063D92DC}" name="Contraseña" dataDxfId="250" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="10" xr3:uid="{082C8AF4-97F4-452C-8F80-F21EF2F991FA}" name="ID Rol" dataDxfId="249"/>
+    <tableColumn id="1" xr3:uid="{851FE67B-C5F3-4094-A11C-923C88F6F300}" name="N.O Documento" dataDxfId="263"/>
+    <tableColumn id="2" xr3:uid="{2632ED65-1042-4D3A-ADC9-D4D0B903999F}" name="ID Documento" dataDxfId="262"/>
+    <tableColumn id="6" xr3:uid="{ABDF7375-83D9-47F3-8016-805F94AE16CC}" name="Primer Nombre" dataDxfId="261"/>
+    <tableColumn id="7" xr3:uid="{C91A11A7-C386-41E9-9560-C1514895842B}" name="Segundo Nombre" dataDxfId="260"/>
+    <tableColumn id="8" xr3:uid="{D75C02DF-B566-48D0-BCEF-1EEAF6C1DBA0}" name="Primer Apellido" dataDxfId="259"/>
+    <tableColumn id="4" xr3:uid="{38E42D0E-DFE7-454C-A189-559E10304022}" name="Segundo Apellido" dataDxfId="258"/>
+    <tableColumn id="9" xr3:uid="{01E3696D-3324-41C5-B5B9-D38D921838B9}" name="Correo 1" dataDxfId="257" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="5" xr3:uid="{6042456D-7E56-4678-804F-8C45063D92DC}" name="Contraseña" dataDxfId="256" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="10" xr3:uid="{082C8AF4-97F4-452C-8F80-F21EF2F991FA}" name="ID Rol" dataDxfId="255"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table49.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="62" xr:uid="{D64A75C0-2E4D-417E-8FE3-64C62E963AC3}" name="Tabla3663" displayName="Tabla3663" ref="B10:H13" totalsRowShown="0" headerRowDxfId="248" dataDxfId="246" headerRowBorderDxfId="247" tableBorderDxfId="245" totalsRowBorderDxfId="244">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="62" xr:uid="{D64A75C0-2E4D-417E-8FE3-64C62E963AC3}" name="Tabla3663" displayName="Tabla3663" ref="B10:H13" totalsRowShown="0" headerRowDxfId="254" dataDxfId="252" headerRowBorderDxfId="253" tableBorderDxfId="251" totalsRowBorderDxfId="250">
   <autoFilter ref="B10:H13" xr:uid="{D64A75C0-2E4D-417E-8FE3-64C62E963AC3}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{09FEE093-6755-4DB6-A784-A08B5B71BE94}" name="Informacion" dataDxfId="243"/>
-    <tableColumn id="5" xr3:uid="{D923D506-CBE3-4555-9AA6-5636AC685DB9}" name="Correo 2" dataDxfId="242" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="6" xr3:uid="{E96DC31F-46B0-4FD8-9756-4E9CFEAB6DF5}" name="Contacto 1" dataDxfId="241"/>
-    <tableColumn id="7" xr3:uid="{D1060EA4-CD2C-4B56-B0E4-22F65F4A2A0A}" name="Contacto 2" dataDxfId="240"/>
-    <tableColumn id="2" xr3:uid="{3706FB50-90FA-4A7F-8159-732869706479}" name="Fecha Nacimiento" dataDxfId="239"/>
-    <tableColumn id="9" xr3:uid="{EB372170-C743-41B9-B564-E1B2CA14C655}" name="Foto" dataDxfId="238"/>
-    <tableColumn id="3" xr3:uid="{2590B856-A1D7-45C7-B59A-3E0FBD6FAA83}" name="N.O Documento" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{09FEE093-6755-4DB6-A784-A08B5B71BE94}" name="Informacion" dataDxfId="249"/>
+    <tableColumn id="5" xr3:uid="{D923D506-CBE3-4555-9AA6-5636AC685DB9}" name="Correo 2" dataDxfId="248" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="6" xr3:uid="{E96DC31F-46B0-4FD8-9756-4E9CFEAB6DF5}" name="Contacto 1" dataDxfId="247"/>
+    <tableColumn id="7" xr3:uid="{D1060EA4-CD2C-4B56-B0E4-22F65F4A2A0A}" name="Contacto 2" dataDxfId="246"/>
+    <tableColumn id="2" xr3:uid="{3706FB50-90FA-4A7F-8159-732869706479}" name="Fecha Nacimiento" dataDxfId="245"/>
+    <tableColumn id="9" xr3:uid="{EB372170-C743-41B9-B564-E1B2CA14C655}" name="Foto" dataDxfId="244"/>
+    <tableColumn id="3" xr3:uid="{2590B856-A1D7-45C7-B59A-3E0FBD6FAA83}" name="N.O Documento" dataDxfId="243"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{3DBDD5EA-EC03-445B-88D5-7D6FFF79B331}" name="Tabla20" displayName="Tabla20" ref="B5:U8" totalsRowShown="0" headerRowDxfId="660" dataDxfId="658" headerRowBorderDxfId="659" tableBorderDxfId="657" totalsRowBorderDxfId="656">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{3DBDD5EA-EC03-445B-88D5-7D6FFF79B331}" name="Tabla20" displayName="Tabla20" ref="B5:U8" totalsRowShown="0" headerRowDxfId="667" dataDxfId="665" headerRowBorderDxfId="666" tableBorderDxfId="664" totalsRowBorderDxfId="663">
   <autoFilter ref="B5:U8" xr:uid="{3DBDD5EA-EC03-445B-88D5-7D6FFF79B331}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{561800E3-1DA2-43F2-815E-B3CA7D19DD0F}" name="N.O Documento" dataDxfId="655"/>
-    <tableColumn id="2" xr3:uid="{6E0A05EF-DBCC-4B85-A53B-683C6C162027}" name="Primer Nombre" dataDxfId="654"/>
-    <tableColumn id="3" xr3:uid="{505A0F7E-84FB-4F2E-9D76-77332524A055}" name="Segundo Nombre" dataDxfId="653"/>
-    <tableColumn id="4" xr3:uid="{0FAD648E-98E1-4AA4-9088-F4B769A1D452}" name="Primer Apellido" dataDxfId="652"/>
-    <tableColumn id="5" xr3:uid="{EF82E1AA-50FF-455D-9F41-AA97E17E0D91}" name="Segundo Apellido" dataDxfId="651"/>
-    <tableColumn id="6" xr3:uid="{7614FB1D-3B04-4DD0-BBA0-502A2459069E}" name="ID Documento" dataDxfId="650"/>
-    <tableColumn id="7" xr3:uid="{1394422F-9D0E-4621-A13F-B007C38936A4}" name="Correo 1" dataDxfId="649" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="8" xr3:uid="{547E3A13-EC21-4279-A834-01CAF1C1CA41}" name="Correo 2" dataDxfId="648" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="9" xr3:uid="{51E9DF50-3AC3-43AF-87AA-01C1DAADF600}" name="Contacto 1" dataDxfId="647"/>
-    <tableColumn id="10" xr3:uid="{CA5BCC39-8A56-40D5-86A1-8E02A9AA6D14}" name="Contacto 2" dataDxfId="646"/>
-    <tableColumn id="11" xr3:uid="{9A67DF33-E118-42B8-858A-708A9F34FF21}" name="ID Rol" dataDxfId="645"/>
-    <tableColumn id="12" xr3:uid="{579F574A-7A09-443E-A02B-C22A8A90A05A}" name="Fecha Nacimiento" dataDxfId="644"/>
-    <tableColumn id="13" xr3:uid="{1B093617-35D5-4B7E-AE86-205C6EDA1BC3}" name="Director Curso" dataDxfId="643"/>
-    <tableColumn id="14" xr3:uid="{C37FA622-470F-459C-B46B-7C1E7B1735F7}" name="Titulo Horario" dataDxfId="642"/>
-    <tableColumn id="15" xr3:uid="{AAF9163B-1AB3-4213-8033-7DB70DC866C3}" name="Imagen Horario" dataDxfId="641"/>
-    <tableColumn id="16" xr3:uid="{1E0ED7E5-A4CE-4FF1-AD38-D22333920007}" name="Descripcion" dataDxfId="640"/>
-    <tableColumn id="18" xr3:uid="{8BB33601-C48C-4ACC-85F2-5BB142BA0422}" name="Jornada" dataDxfId="639"/>
-    <tableColumn id="19" xr3:uid="{15091081-BCD9-4733-8EA6-5753A623E774}" name="ID Curso 1" dataDxfId="638"/>
-    <tableColumn id="20" xr3:uid="{8F11227C-3440-41AE-A7D6-451C322577EE}" name="ID Curso 2" dataDxfId="637"/>
-    <tableColumn id="21" xr3:uid="{1DAED5F5-17F5-4CAD-8AFB-258972D9B61B}" name="Grado" dataDxfId="636"/>
+    <tableColumn id="1" xr3:uid="{561800E3-1DA2-43F2-815E-B3CA7D19DD0F}" name="N.O Documento" dataDxfId="662"/>
+    <tableColumn id="2" xr3:uid="{6E0A05EF-DBCC-4B85-A53B-683C6C162027}" name="Primer Nombre" dataDxfId="661"/>
+    <tableColumn id="3" xr3:uid="{505A0F7E-84FB-4F2E-9D76-77332524A055}" name="Segundo Nombre" dataDxfId="660"/>
+    <tableColumn id="4" xr3:uid="{0FAD648E-98E1-4AA4-9088-F4B769A1D452}" name="Primer Apellido" dataDxfId="659"/>
+    <tableColumn id="5" xr3:uid="{EF82E1AA-50FF-455D-9F41-AA97E17E0D91}" name="Segundo Apellido" dataDxfId="658"/>
+    <tableColumn id="6" xr3:uid="{7614FB1D-3B04-4DD0-BBA0-502A2459069E}" name="ID Documento" dataDxfId="657"/>
+    <tableColumn id="7" xr3:uid="{1394422F-9D0E-4621-A13F-B007C38936A4}" name="Correo 1" dataDxfId="656" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="8" xr3:uid="{547E3A13-EC21-4279-A834-01CAF1C1CA41}" name="Correo 2" dataDxfId="655" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="9" xr3:uid="{51E9DF50-3AC3-43AF-87AA-01C1DAADF600}" name="Contacto 1" dataDxfId="654"/>
+    <tableColumn id="10" xr3:uid="{CA5BCC39-8A56-40D5-86A1-8E02A9AA6D14}" name="Contacto 2" dataDxfId="653"/>
+    <tableColumn id="11" xr3:uid="{9A67DF33-E118-42B8-858A-708A9F34FF21}" name="ID Rol" dataDxfId="652"/>
+    <tableColumn id="12" xr3:uid="{579F574A-7A09-443E-A02B-C22A8A90A05A}" name="Fecha Nacimiento" dataDxfId="651"/>
+    <tableColumn id="13" xr3:uid="{1B093617-35D5-4B7E-AE86-205C6EDA1BC3}" name="Director Curso" dataDxfId="650"/>
+    <tableColumn id="14" xr3:uid="{C37FA622-470F-459C-B46B-7C1E7B1735F7}" name="Titulo Horario" dataDxfId="649"/>
+    <tableColumn id="15" xr3:uid="{AAF9163B-1AB3-4213-8033-7DB70DC866C3}" name="Imagen Horario" dataDxfId="648"/>
+    <tableColumn id="16" xr3:uid="{1E0ED7E5-A4CE-4FF1-AD38-D22333920007}" name="Descripcion" dataDxfId="647"/>
+    <tableColumn id="18" xr3:uid="{8BB33601-C48C-4ACC-85F2-5BB142BA0422}" name="Jornada" dataDxfId="646"/>
+    <tableColumn id="19" xr3:uid="{15091081-BCD9-4733-8EA6-5753A623E774}" name="ID Curso 1" dataDxfId="645"/>
+    <tableColumn id="20" xr3:uid="{8F11227C-3440-41AE-A7D6-451C322577EE}" name="ID Curso 2" dataDxfId="644"/>
+    <tableColumn id="21" xr3:uid="{1DAED5F5-17F5-4CAD-8AFB-258972D9B61B}" name="Grado" dataDxfId="643"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table50.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="68" xr:uid="{D31D7735-74EE-444C-AC0A-BB2304E67D61}" name="Tabla294169" displayName="Tabla294169" ref="H17:K20" totalsRowShown="0" headerRowDxfId="237" dataDxfId="235" headerRowBorderDxfId="236" tableBorderDxfId="234" totalsRowBorderDxfId="233">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="68" xr:uid="{D31D7735-74EE-444C-AC0A-BB2304E67D61}" name="Tabla294169" displayName="Tabla294169" ref="H17:K20" totalsRowShown="0" headerRowDxfId="242" dataDxfId="240" headerRowBorderDxfId="241" tableBorderDxfId="239" totalsRowBorderDxfId="238">
   <autoFilter ref="H17:K20" xr:uid="{D31D7735-74EE-444C-AC0A-BB2304E67D61}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{52B396CC-68D2-48DB-B0DA-F0B39BBFBE6A}" name="ID Curso" dataDxfId="232"/>
-    <tableColumn id="2" xr3:uid="{C698F786-B166-416F-88D7-058EE365E0E4}" name="Nombre Curso" dataDxfId="231"/>
-    <tableColumn id="4" xr3:uid="{65638558-CBF7-4A04-91EB-AD187D0D078B}" name="ID Jornada" dataDxfId="230"/>
-    <tableColumn id="5" xr3:uid="{78987584-FA28-4103-9176-AD5CC73ED7BC}" name="ID Grado" dataDxfId="229"/>
+    <tableColumn id="1" xr3:uid="{52B396CC-68D2-48DB-B0DA-F0B39BBFBE6A}" name="ID Curso" dataDxfId="237"/>
+    <tableColumn id="2" xr3:uid="{C698F786-B166-416F-88D7-058EE365E0E4}" name="Nombre Curso" dataDxfId="236"/>
+    <tableColumn id="4" xr3:uid="{65638558-CBF7-4A04-91EB-AD187D0D078B}" name="ID Jornada" dataDxfId="235"/>
+    <tableColumn id="5" xr3:uid="{78987584-FA28-4103-9176-AD5CC73ED7BC}" name="ID Grado" dataDxfId="234"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table51.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{05DEF17C-367E-4569-9FA4-6DEC620E884D}" name="Tabla34404370" displayName="Tabla34404370" ref="B17:C21" totalsRowShown="0" headerRowDxfId="228" dataDxfId="226" headerRowBorderDxfId="227" tableBorderDxfId="225" totalsRowBorderDxfId="224">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="69" xr:uid="{05DEF17C-367E-4569-9FA4-6DEC620E884D}" name="Tabla34404370" displayName="Tabla34404370" ref="B17:C21" totalsRowShown="0" headerRowDxfId="233" dataDxfId="231" headerRowBorderDxfId="232" tableBorderDxfId="230" totalsRowBorderDxfId="229">
   <autoFilter ref="B17:C21" xr:uid="{05DEF17C-367E-4569-9FA4-6DEC620E884D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{CED531A4-B01B-4A6F-8D3A-6067AC5F017C}" name="ID Rol" dataDxfId="223"/>
-    <tableColumn id="2" xr3:uid="{9283E436-717C-4B52-9DE6-A174FD439053}" name="Rol" dataDxfId="222"/>
+    <tableColumn id="1" xr3:uid="{CED531A4-B01B-4A6F-8D3A-6067AC5F017C}" name="ID Rol" dataDxfId="228"/>
+    <tableColumn id="2" xr3:uid="{9283E436-717C-4B52-9DE6-A174FD439053}" name="Rol" dataDxfId="227"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table52.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="70" xr:uid="{EE816A73-CC59-4799-85BE-02744D9ACAB2}" name="Tabla2739424471" displayName="Tabla2739424471" ref="E17:F20" totalsRowShown="0" headerRowDxfId="221" dataDxfId="219" headerRowBorderDxfId="220" tableBorderDxfId="218" totalsRowBorderDxfId="217">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="70" xr:uid="{EE816A73-CC59-4799-85BE-02744D9ACAB2}" name="Tabla2739424471" displayName="Tabla2739424471" ref="E17:F20" totalsRowShown="0" headerRowDxfId="226" dataDxfId="224" headerRowBorderDxfId="225" tableBorderDxfId="223" totalsRowBorderDxfId="222">
   <autoFilter ref="E17:F20" xr:uid="{EE816A73-CC59-4799-85BE-02744D9ACAB2}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{53DF8DBF-134D-4CB4-A89D-6E16811445D3}" name="ID Documento" dataDxfId="216"/>
-    <tableColumn id="2" xr3:uid="{4F2BE242-2696-4C6F-B38A-AE24001608C1}" name="Tipo Documento" dataDxfId="215"/>
+    <tableColumn id="1" xr3:uid="{53DF8DBF-134D-4CB4-A89D-6E16811445D3}" name="ID Documento" dataDxfId="221"/>
+    <tableColumn id="2" xr3:uid="{4F2BE242-2696-4C6F-B38A-AE24001608C1}" name="Tipo Documento" dataDxfId="220"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table53.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="71" xr:uid="{C6044070-C0F9-4732-A51D-F247B487EB4F}" name="Tabla4772" displayName="Tabla4772" ref="B25:E28" totalsRowShown="0" headerRowDxfId="214" dataDxfId="212" headerRowBorderDxfId="213" tableBorderDxfId="211" totalsRowBorderDxfId="210">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="71" xr:uid="{C6044070-C0F9-4732-A51D-F247B487EB4F}" name="Tabla4772" displayName="Tabla4772" ref="B25:E28" totalsRowShown="0" headerRowDxfId="219" dataDxfId="217" headerRowBorderDxfId="218" tableBorderDxfId="216" totalsRowBorderDxfId="215">
   <autoFilter ref="B25:E28" xr:uid="{C6044070-C0F9-4732-A51D-F247B487EB4F}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C3CFE7FC-DB9F-446E-B781-6FC7F1A0014A}" name="ID Horario" dataDxfId="209"/>
-    <tableColumn id="2" xr3:uid="{3A85A481-1F1D-4E45-A793-9B5D7F0C79B1}" name="Titulo Horario" dataDxfId="208"/>
-    <tableColumn id="3" xr3:uid="{E243F55A-F3AA-4E7C-AC85-916EE50968CC}" name="Imagen Horario" dataDxfId="207"/>
-    <tableColumn id="4" xr3:uid="{3B5CA442-9EE0-4901-8F08-9D3F585A6F39}" name="Descripcion" dataDxfId="206"/>
+    <tableColumn id="1" xr3:uid="{C3CFE7FC-DB9F-446E-B781-6FC7F1A0014A}" name="ID Horario" dataDxfId="214"/>
+    <tableColumn id="2" xr3:uid="{3A85A481-1F1D-4E45-A793-9B5D7F0C79B1}" name="Titulo Horario" dataDxfId="213"/>
+    <tableColumn id="3" xr3:uid="{E243F55A-F3AA-4E7C-AC85-916EE50968CC}" name="Imagen Horario" dataDxfId="212"/>
+    <tableColumn id="4" xr3:uid="{3B5CA442-9EE0-4901-8F08-9D3F585A6F39}" name="Descripcion" dataDxfId="211"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table54.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="72" xr:uid="{F80E1943-62E7-4DDC-A1BD-C067BDA2EF34}" name="Tabla3873" displayName="Tabla3873" ref="H25:J28" totalsRowShown="0" headerRowDxfId="205" dataDxfId="203" headerRowBorderDxfId="204" tableBorderDxfId="202" totalsRowBorderDxfId="201">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="72" xr:uid="{F80E1943-62E7-4DDC-A1BD-C067BDA2EF34}" name="Tabla3873" displayName="Tabla3873" ref="H25:J28" totalsRowShown="0" headerRowDxfId="210" dataDxfId="208" headerRowBorderDxfId="209" tableBorderDxfId="207" totalsRowBorderDxfId="206">
   <autoFilter ref="H25:J28" xr:uid="{F80E1943-62E7-4DDC-A1BD-C067BDA2EF34}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{FF6CD945-688A-45EE-BE8D-05B4CEA81F85}" name="Curso" dataDxfId="200"/>
-    <tableColumn id="3" xr3:uid="{7AB70B95-F4A7-4AD9-9C2A-A7C49B9636BF}" name="ID Profesor" dataDxfId="199"/>
-    <tableColumn id="2" xr3:uid="{8DE15A01-F940-42C5-AB51-9F5CDA1A9A38}" name="ID Horario" dataDxfId="198"/>
+    <tableColumn id="1" xr3:uid="{FF6CD945-688A-45EE-BE8D-05B4CEA81F85}" name="Curso" dataDxfId="205"/>
+    <tableColumn id="3" xr3:uid="{7AB70B95-F4A7-4AD9-9C2A-A7C49B9636BF}" name="ID Profesor" dataDxfId="204"/>
+    <tableColumn id="2" xr3:uid="{8DE15A01-F940-42C5-AB51-9F5CDA1A9A38}" name="ID Horario" dataDxfId="203"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table55.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="73" xr:uid="{4E6AE856-EAAC-4CEE-B992-610251E38B51}" name="Tabla3974" displayName="Tabla3974" ref="G25:G28" totalsRowShown="0" headerRowDxfId="197" dataDxfId="196">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="73" xr:uid="{4E6AE856-EAAC-4CEE-B992-610251E38B51}" name="Tabla3974" displayName="Tabla3974" ref="G25:G28" totalsRowShown="0" headerRowDxfId="202" dataDxfId="201">
   <autoFilter ref="G25:G28" xr:uid="{4E6AE856-EAAC-4CEE-B992-610251E38B51}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{FBEDA0E7-22BA-4501-AF73-15F5489C7A72}" name="ID Horario" dataDxfId="195"/>
+    <tableColumn id="1" xr3:uid="{FBEDA0E7-22BA-4501-AF73-15F5489C7A72}" name="ID Horario" dataDxfId="200"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table56.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{7C9D0BAA-6654-4D73-BA85-4DFD2A609059}" name="Tabla445675" displayName="Tabla445675" ref="J10:K13" totalsRowShown="0" headerRowDxfId="194" dataDxfId="192" headerRowBorderDxfId="193" tableBorderDxfId="191" totalsRowBorderDxfId="190">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="74" xr:uid="{7C9D0BAA-6654-4D73-BA85-4DFD2A609059}" name="Tabla445675" displayName="Tabla445675" ref="J10:K13" totalsRowShown="0" headerRowDxfId="199" dataDxfId="197" headerRowBorderDxfId="198" tableBorderDxfId="196" totalsRowBorderDxfId="195">
   <autoFilter ref="J10:K13" xr:uid="{7C9D0BAA-6654-4D73-BA85-4DFD2A609059}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9B80FAAC-746C-405C-8441-77F2AF737CB4}" name="ID Curso" dataDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{A8D196AB-BE98-489B-A761-D842A18486DE}" name="Miembros" dataDxfId="188"/>
+    <tableColumn id="1" xr3:uid="{9B80FAAC-746C-405C-8441-77F2AF737CB4}" name="ID Curso" dataDxfId="194"/>
+    <tableColumn id="2" xr3:uid="{A8D196AB-BE98-489B-A761-D842A18486DE}" name="Miembros" dataDxfId="193"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table57.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="75" xr:uid="{B8CFA8BA-4CC6-45A6-8CEE-BBCE4C1CD86F}" name="Tabla356576" displayName="Tabla356576" ref="M10:O13" totalsRowShown="0" headerRowDxfId="187" dataDxfId="185" headerRowBorderDxfId="186" tableBorderDxfId="184" totalsRowBorderDxfId="183">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="75" xr:uid="{B8CFA8BA-4CC6-45A6-8CEE-BBCE4C1CD86F}" name="Tabla356576" displayName="Tabla356576" ref="M10:O13" totalsRowShown="0" headerRowDxfId="192" dataDxfId="190" headerRowBorderDxfId="191" tableBorderDxfId="189" totalsRowBorderDxfId="188">
   <autoFilter ref="M10:O13" xr:uid="{B8CFA8BA-4CC6-45A6-8CEE-BBCE4C1CD86F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{C901B504-0423-4002-93E7-A611AD49BB6B}" name="ID Materia" dataDxfId="182"/>
-    <tableColumn id="2" xr3:uid="{26747C08-082A-423F-A49E-68FCAA29ABF4}" name="Nombre Materia" dataDxfId="181"/>
-    <tableColumn id="3" xr3:uid="{9C99F0F6-8B2F-413F-A288-C34E7C795799}" name="Descripcion" dataDxfId="180"/>
+    <tableColumn id="1" xr3:uid="{C901B504-0423-4002-93E7-A611AD49BB6B}" name="ID Materia" dataDxfId="187"/>
+    <tableColumn id="2" xr3:uid="{26747C08-082A-423F-A49E-68FCAA29ABF4}" name="Nombre Materia" dataDxfId="186"/>
+    <tableColumn id="3" xr3:uid="{9C99F0F6-8B2F-413F-A288-C34E7C795799}" name="Descripcion" dataDxfId="185"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table58.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{382EFBB7-1466-4DBE-9199-9CC4AAF37FB2}" name="Tabla3046455077" displayName="Tabla3046455077" ref="M17:N20" totalsRowShown="0" headerRowDxfId="179" dataDxfId="177" headerRowBorderDxfId="178" tableBorderDxfId="176" totalsRowBorderDxfId="175">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="76" xr:uid="{382EFBB7-1466-4DBE-9199-9CC4AAF37FB2}" name="Tabla3046455077" displayName="Tabla3046455077" ref="M17:N20" totalsRowShown="0" headerRowDxfId="184" dataDxfId="182" headerRowBorderDxfId="183" tableBorderDxfId="181" totalsRowBorderDxfId="180">
   <autoFilter ref="M17:N20" xr:uid="{382EFBB7-1466-4DBE-9199-9CC4AAF37FB2}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2B5B92ED-ADFC-4D6F-A82B-9B0AC2CBF89B}" name="ID Grado" dataDxfId="174"/>
-    <tableColumn id="2" xr3:uid="{A2E2121B-2960-4413-989E-64FF66F49E67}" name="Grado" dataDxfId="173"/>
+    <tableColumn id="1" xr3:uid="{2B5B92ED-ADFC-4D6F-A82B-9B0AC2CBF89B}" name="ID Grado" dataDxfId="179"/>
+    <tableColumn id="2" xr3:uid="{A2E2121B-2960-4413-989E-64FF66F49E67}" name="Grado" dataDxfId="178"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table59.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="77" xr:uid="{12405811-2916-4E90-9D5F-E51B99FB858B}" name="Tabla2847495378" displayName="Tabla2847495378" ref="P17:Q19" totalsRowShown="0" headerRowDxfId="172" dataDxfId="170" headerRowBorderDxfId="171" tableBorderDxfId="169" totalsRowBorderDxfId="168">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="77" xr:uid="{12405811-2916-4E90-9D5F-E51B99FB858B}" name="Tabla2847495378" displayName="Tabla2847495378" ref="P17:Q19" totalsRowShown="0" headerRowDxfId="177" dataDxfId="175" headerRowBorderDxfId="176" tableBorderDxfId="174" totalsRowBorderDxfId="173">
   <autoFilter ref="P17:Q19" xr:uid="{12405811-2916-4E90-9D5F-E51B99FB858B}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DEB73736-224E-4907-9ED9-431A7BC7B325}" name="ID Jornada" dataDxfId="167"/>
-    <tableColumn id="2" xr3:uid="{D89F12EC-5AB7-475F-BC19-34F2ECAD1694}" name="Jornada" dataDxfId="166"/>
+    <tableColumn id="1" xr3:uid="{DEB73736-224E-4907-9ED9-431A7BC7B325}" name="ID Jornada" dataDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{D89F12EC-5AB7-475F-BC19-34F2ECAD1694}" name="Jornada" dataDxfId="171"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{AFB62245-93EF-4AC6-A95A-E5D43EBD5F5A}" name="Tabla21" displayName="Tabla21" ref="B12:O15" totalsRowShown="0" headerRowDxfId="635" dataDxfId="634">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{AFB62245-93EF-4AC6-A95A-E5D43EBD5F5A}" name="Tabla21" displayName="Tabla21" ref="B12:O15" totalsRowShown="0" headerRowDxfId="642" dataDxfId="641">
   <autoFilter ref="B12:O15" xr:uid="{AFB62245-93EF-4AC6-A95A-E5D43EBD5F5A}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{3E16F56D-B67E-4784-8C0D-6D43066A709B}" name="ID Aula" dataDxfId="633"/>
-    <tableColumn id="2" xr3:uid="{91C5CEE5-5608-4CE4-9544-F63A8585D08E}" name="Nombre Aula" dataDxfId="632"/>
-    <tableColumn id="3" xr3:uid="{251A64CE-A0D9-49A7-B413-7A5EFC01B22F}" name="ID Curso" dataDxfId="631"/>
-    <tableColumn id="4" xr3:uid="{56F383C5-7E75-4B6E-B84C-731CFA031AD4}" name="ID Materia" dataDxfId="630"/>
-    <tableColumn id="5" xr3:uid="{E88FA1AE-0271-44DF-9AC7-F5A26C9BBF28}" name="ID Profesor" dataDxfId="629"/>
-    <tableColumn id="6" xr3:uid="{2DF9DF7B-1210-4059-9B98-73B5A4EBE7AC}" name="Tareas" dataDxfId="628"/>
-    <tableColumn id="7" xr3:uid="{C8D64524-4E41-45B9-B5CE-EFF94BB244D4}" name="Descripcion" dataDxfId="627"/>
-    <tableColumn id="8" xr3:uid="{7A7F2D7C-3047-4B52-920A-F1A694377D29}" name="Tema" dataDxfId="626"/>
-    <tableColumn id="9" xr3:uid="{CD998114-FF29-43EA-8418-09B8A6CF6D00}" name="Archivo" dataDxfId="625"/>
-    <tableColumn id="10" xr3:uid="{D0B9C00C-81A6-4A0F-BA10-5AF02511FE85}" name="Fecha Entrega" dataDxfId="624"/>
-    <tableColumn id="12" xr3:uid="{048C235A-31F9-4C64-9CCD-F388DEE2BACA}" name="Anuncio" dataDxfId="623"/>
-    <tableColumn id="13" xr3:uid="{E2F7A130-FB74-4097-91BB-DADF3BF4A4E8}" name="Descripcion Anuncio" dataDxfId="622"/>
-    <tableColumn id="14" xr3:uid="{D84A0F63-3AD0-490D-A27D-9A0113C12368}" name="Archivo Anuncio" dataDxfId="621"/>
-    <tableColumn id="15" xr3:uid="{7D8D4A19-0407-41DB-8C50-ADBE06F1DABE}" name="Fecha" dataDxfId="620"/>
+    <tableColumn id="1" xr3:uid="{3E16F56D-B67E-4784-8C0D-6D43066A709B}" name="ID Aula" dataDxfId="640"/>
+    <tableColumn id="2" xr3:uid="{91C5CEE5-5608-4CE4-9544-F63A8585D08E}" name="Nombre Aula" dataDxfId="639"/>
+    <tableColumn id="3" xr3:uid="{251A64CE-A0D9-49A7-B413-7A5EFC01B22F}" name="ID Curso" dataDxfId="638"/>
+    <tableColumn id="4" xr3:uid="{56F383C5-7E75-4B6E-B84C-731CFA031AD4}" name="ID Materia" dataDxfId="637"/>
+    <tableColumn id="5" xr3:uid="{E88FA1AE-0271-44DF-9AC7-F5A26C9BBF28}" name="ID Profesor" dataDxfId="636"/>
+    <tableColumn id="6" xr3:uid="{2DF9DF7B-1210-4059-9B98-73B5A4EBE7AC}" name="Tareas" dataDxfId="635"/>
+    <tableColumn id="7" xr3:uid="{C8D64524-4E41-45B9-B5CE-EFF94BB244D4}" name="Descripcion" dataDxfId="634"/>
+    <tableColumn id="8" xr3:uid="{7A7F2D7C-3047-4B52-920A-F1A694377D29}" name="Tema" dataDxfId="633"/>
+    <tableColumn id="9" xr3:uid="{CD998114-FF29-43EA-8418-09B8A6CF6D00}" name="Archivo" dataDxfId="632"/>
+    <tableColumn id="10" xr3:uid="{D0B9C00C-81A6-4A0F-BA10-5AF02511FE85}" name="Fecha Entrega" dataDxfId="631"/>
+    <tableColumn id="12" xr3:uid="{048C235A-31F9-4C64-9CCD-F388DEE2BACA}" name="Anuncio" dataDxfId="630"/>
+    <tableColumn id="13" xr3:uid="{E2F7A130-FB74-4097-91BB-DADF3BF4A4E8}" name="Descripcion Anuncio" dataDxfId="629"/>
+    <tableColumn id="14" xr3:uid="{D84A0F63-3AD0-490D-A27D-9A0113C12368}" name="Archivo Anuncio" dataDxfId="628"/>
+    <tableColumn id="15" xr3:uid="{7D8D4A19-0407-41DB-8C50-ADBE06F1DABE}" name="Fecha" dataDxfId="627"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table60.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{5D0EDFAD-EEEA-4D2A-9A20-6DF91EC76FF1}" name="Tabla4145" displayName="Tabla4145" ref="B39:H42" totalsRowShown="0" headerRowDxfId="165" dataDxfId="163" headerRowBorderDxfId="164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{5D0EDFAD-EEEA-4D2A-9A20-6DF91EC76FF1}" name="Tabla4145" displayName="Tabla4145" ref="B39:H42" totalsRowShown="0" headerRowDxfId="170" dataDxfId="168" headerRowBorderDxfId="169">
   <autoFilter ref="B39:H42" xr:uid="{5D0EDFAD-EEEA-4D2A-9A20-6DF91EC76FF1}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{64C3D65A-CBB5-4FE0-8266-68C6EBFE2761}" name="ID Anuncios" dataDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{67606ABD-9032-4188-88B5-264974BA1379}" name="Titulo" dataDxfId="161"/>
-    <tableColumn id="3" xr3:uid="{BB5ACA5B-2C27-4A91-BAE2-84177191C8FB}" name="Descripcion" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{5325DB20-1891-47C1-B3E7-959A75ECC380}" name="Archivo Anuncio" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{0A48D784-4341-4CB8-8040-63BD87CBDFAE}" name="Fecha" dataDxfId="158"/>
-    <tableColumn id="7" xr3:uid="{9A0E83C5-6363-4C86-A010-1A37C8D84A6A}" name="ID Aula" dataDxfId="157"/>
-    <tableColumn id="6" xr3:uid="{0151CCFE-CF43-429B-9DF3-83C5D56479FE}" name="ID Usuario" dataDxfId="156"/>
+    <tableColumn id="1" xr3:uid="{64C3D65A-CBB5-4FE0-8266-68C6EBFE2761}" name="ID Anuncios" dataDxfId="167"/>
+    <tableColumn id="2" xr3:uid="{67606ABD-9032-4188-88B5-264974BA1379}" name="Titulo" dataDxfId="166"/>
+    <tableColumn id="3" xr3:uid="{BB5ACA5B-2C27-4A91-BAE2-84177191C8FB}" name="Descripcion" dataDxfId="165"/>
+    <tableColumn id="4" xr3:uid="{5325DB20-1891-47C1-B3E7-959A75ECC380}" name="Archivo Anuncio" dataDxfId="164"/>
+    <tableColumn id="5" xr3:uid="{0A48D784-4341-4CB8-8040-63BD87CBDFAE}" name="Fecha" dataDxfId="163"/>
+    <tableColumn id="7" xr3:uid="{9A0E83C5-6363-4C86-A010-1A37C8D84A6A}" name="ID Aula" dataDxfId="162"/>
+    <tableColumn id="6" xr3:uid="{0151CCFE-CF43-429B-9DF3-83C5D56479FE}" name="ID Usuario" dataDxfId="161"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table61.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{3B7812E8-BD5D-4787-80EA-153C319C463A}" name="Tabla5147" displayName="Tabla5147" ref="Q39:W42" totalsRowShown="0" headerRowDxfId="155" dataDxfId="153" headerRowBorderDxfId="154">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{3B7812E8-BD5D-4787-80EA-153C319C463A}" name="Tabla5147" displayName="Tabla5147" ref="Q39:W42" totalsRowShown="0" headerRowDxfId="160" dataDxfId="158" headerRowBorderDxfId="159">
   <autoFilter ref="Q39:W42" xr:uid="{3B7812E8-BD5D-4787-80EA-153C319C463A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3FCDBA56-8C41-4E78-BC9B-08574210A510}" name="ID Trabajos" dataDxfId="152"/>
-    <tableColumn id="2" xr3:uid="{92868082-ACC5-4B8F-8A5E-4756A3B73E63}" name="Tema" dataDxfId="151"/>
-    <tableColumn id="3" xr3:uid="{86B3B348-D99A-4F79-84BB-7264C7EAED06}" name="Titulo Trabajo" dataDxfId="150"/>
-    <tableColumn id="4" xr3:uid="{324D48B6-7BBF-47BA-BA79-2DFEE1ADCBA5}" name="Descripcion" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{F69CE0DF-1458-4BC9-8A79-D7064CAC1F61}" name="Fecha Entrega" dataDxfId="148"/>
-    <tableColumn id="6" xr3:uid="{49008FB2-AE39-4D4D-9BA0-F75C124EAB91}" name="Archivo" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{F4CCC61B-F5C6-4821-8725-768B2BB3F2CA}" name="ID Aula" dataDxfId="146"/>
+    <tableColumn id="1" xr3:uid="{3FCDBA56-8C41-4E78-BC9B-08574210A510}" name="ID Trabajos" dataDxfId="157"/>
+    <tableColumn id="2" xr3:uid="{92868082-ACC5-4B8F-8A5E-4756A3B73E63}" name="Tema" dataDxfId="156"/>
+    <tableColumn id="3" xr3:uid="{86B3B348-D99A-4F79-84BB-7264C7EAED06}" name="Titulo Trabajo" dataDxfId="155"/>
+    <tableColumn id="4" xr3:uid="{324D48B6-7BBF-47BA-BA79-2DFEE1ADCBA5}" name="Descripcion" dataDxfId="154"/>
+    <tableColumn id="5" xr3:uid="{F69CE0DF-1458-4BC9-8A79-D7064CAC1F61}" name="Fecha Entrega" dataDxfId="153"/>
+    <tableColumn id="6" xr3:uid="{49008FB2-AE39-4D4D-9BA0-F75C124EAB91}" name="Archivo" dataDxfId="152"/>
+    <tableColumn id="7" xr3:uid="{F4CCC61B-F5C6-4821-8725-768B2BB3F2CA}" name="ID Aula" dataDxfId="151"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table62.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="48" xr:uid="{79F0B324-423F-45C4-A260-00FA88F11BD4}" name="Tabla5349" displayName="Tabla5349" ref="Y39:AB42" totalsRowShown="0" headerRowDxfId="145" dataDxfId="143" headerRowBorderDxfId="144" tableBorderDxfId="142" totalsRowBorderDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="48" xr:uid="{79F0B324-423F-45C4-A260-00FA88F11BD4}" name="Tabla5349" displayName="Tabla5349" ref="Y39:AB42" totalsRowShown="0" headerRowDxfId="150" dataDxfId="148" headerRowBorderDxfId="149" tableBorderDxfId="147" totalsRowBorderDxfId="146">
   <autoFilter ref="Y39:AB42" xr:uid="{79F0B324-423F-45C4-A260-00FA88F11BD4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F3597883-F690-44C7-AF6A-49728F6F6036}" name="ID Calificacion" dataDxfId="140"/>
-    <tableColumn id="2" xr3:uid="{2A32C5A4-1463-480E-8F62-5ABCFDD30A95}" name="ID Alumno" dataDxfId="139"/>
-    <tableColumn id="3" xr3:uid="{451077B5-F1EE-4A77-B237-CE09C3F20B04}" name="ID Trabajos" dataDxfId="138"/>
-    <tableColumn id="4" xr3:uid="{4A442456-77FB-486A-B49B-927CFBA37733}" name="Nota" dataDxfId="137"/>
+    <tableColumn id="1" xr3:uid="{F3597883-F690-44C7-AF6A-49728F6F6036}" name="ID Calificacion" dataDxfId="145"/>
+    <tableColumn id="2" xr3:uid="{2A32C5A4-1463-480E-8F62-5ABCFDD30A95}" name="ID Alumno" dataDxfId="144"/>
+    <tableColumn id="3" xr3:uid="{451077B5-F1EE-4A77-B237-CE09C3F20B04}" name="ID Trabajos" dataDxfId="143"/>
+    <tableColumn id="4" xr3:uid="{4A442456-77FB-486A-B49B-927CFBA37733}" name="Nota" dataDxfId="142"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table63.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="60" xr:uid="{41935AFA-4A92-469A-9EED-554D6D74495C}" name="Tabla245561" displayName="Tabla245561" ref="B46:E49" totalsRowShown="0" headerRowDxfId="136" dataDxfId="134" headerRowBorderDxfId="135" tableBorderDxfId="133" totalsRowBorderDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="60" xr:uid="{41935AFA-4A92-469A-9EED-554D6D74495C}" name="Tabla245561" displayName="Tabla245561" ref="B46:E49" totalsRowShown="0" headerRowDxfId="141" dataDxfId="139" headerRowBorderDxfId="140" tableBorderDxfId="138" totalsRowBorderDxfId="137">
   <autoFilter ref="B46:E49" xr:uid="{41935AFA-4A92-469A-9EED-554D6D74495C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A57E5829-FE7F-4C71-9605-4FB93AB3D4F4}" name="ID Notas" dataDxfId="131"/>
-    <tableColumn id="2" xr3:uid="{F5B99937-E1F8-4CEB-9E76-E07E5AED919F}" name="ID Curso" dataDxfId="130"/>
-    <tableColumn id="6" xr3:uid="{8A9C3E0C-26AD-465A-A1D4-8BA385EB2343}" name="ID Nota Final" dataDxfId="129"/>
-    <tableColumn id="3" xr3:uid="{BD6A2261-5825-4A56-A1AB-F4F28D04B6A3}" name="ID Planilla" dataDxfId="128"/>
+    <tableColumn id="1" xr3:uid="{A57E5829-FE7F-4C71-9605-4FB93AB3D4F4}" name="ID Notas" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{F5B99937-E1F8-4CEB-9E76-E07E5AED919F}" name="ID Curso" dataDxfId="135"/>
+    <tableColumn id="6" xr3:uid="{8A9C3E0C-26AD-465A-A1D4-8BA385EB2343}" name="ID Nota Final" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{BD6A2261-5825-4A56-A1AB-F4F28D04B6A3}" name="ID Planilla" dataDxfId="133"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table64.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{5EB4A6D8-A6E0-4FA1-ACA3-6058ECAB90AB}" name="Tabla235779" displayName="Tabla235779" ref="B53:D56" totalsRowShown="0" headerRowDxfId="127" dataDxfId="125" headerRowBorderDxfId="126" tableBorderDxfId="124" totalsRowBorderDxfId="123">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="78" xr:uid="{5EB4A6D8-A6E0-4FA1-ACA3-6058ECAB90AB}" name="Tabla235779" displayName="Tabla235779" ref="B53:D56" totalsRowShown="0" headerRowDxfId="132" dataDxfId="130" headerRowBorderDxfId="131" tableBorderDxfId="129" totalsRowBorderDxfId="128">
   <autoFilter ref="B53:D56" xr:uid="{5EB4A6D8-A6E0-4FA1-ACA3-6058ECAB90AB}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{8753FDF1-1142-4257-8A1A-2103A09A0E47}" name="ID Planilla" dataDxfId="122"/>
-    <tableColumn id="2" xr3:uid="{38EE62A7-BFF0-474F-8F6C-67CBC682425E}" name="Nombre Planilla" dataDxfId="121"/>
-    <tableColumn id="3" xr3:uid="{80D89775-451C-465C-B53E-8F6D5D4D30D9}" name="ID Periodo" dataDxfId="120"/>
+    <tableColumn id="1" xr3:uid="{8753FDF1-1142-4257-8A1A-2103A09A0E47}" name="ID Planilla" dataDxfId="127"/>
+    <tableColumn id="2" xr3:uid="{38EE62A7-BFF0-474F-8F6C-67CBC682425E}" name="Nombre Planilla" dataDxfId="126"/>
+    <tableColumn id="3" xr3:uid="{80D89775-451C-465C-B53E-8F6D5D4D30D9}" name="ID Periodo" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table65.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="81" xr:uid="{B9539AA5-C133-444E-BE9B-F846DF706BEE}" name="Tabla315982" displayName="Tabla315982" ref="F53:G57" totalsRowShown="0" headerRowDxfId="119" dataDxfId="117" headerRowBorderDxfId="118" tableBorderDxfId="116" totalsRowBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="81" xr:uid="{B9539AA5-C133-444E-BE9B-F846DF706BEE}" name="Tabla315982" displayName="Tabla315982" ref="F53:G57" totalsRowShown="0" headerRowDxfId="124" dataDxfId="122" headerRowBorderDxfId="123" tableBorderDxfId="121" totalsRowBorderDxfId="120">
   <autoFilter ref="F53:G57" xr:uid="{B9539AA5-C133-444E-BE9B-F846DF706BEE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A4834879-059C-4D4C-A769-460D803918F5}" name="ID Perido" dataDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{4717E88F-53F5-46B8-89BF-CF128B9D3CD4}" name="Periodo" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{A4834879-059C-4D4C-A769-460D803918F5}" name="ID Perido" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{4717E88F-53F5-46B8-89BF-CF128B9D3CD4}" name="Periodo" dataDxfId="118"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table66.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="82" xr:uid="{5D204371-67A4-4417-87C0-7083224956B9}" name="Tabla5983" displayName="Tabla5983" ref="B60:I63" totalsRowShown="0" headerRowDxfId="112" dataDxfId="110" headerRowBorderDxfId="111" tableBorderDxfId="109" totalsRowBorderDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="82" xr:uid="{5D204371-67A4-4417-87C0-7083224956B9}" name="Tabla5983" displayName="Tabla5983" ref="B60:I63" totalsRowShown="0" headerRowDxfId="117" dataDxfId="115" headerRowBorderDxfId="116" tableBorderDxfId="114" totalsRowBorderDxfId="113">
   <autoFilter ref="B60:I63" xr:uid="{5D204371-67A4-4417-87C0-7083224956B9}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{68514C17-60C3-4A0D-A349-2C66A403B3C1}" name="ID Boletin" dataDxfId="107"/>
-    <tableColumn id="2" xr3:uid="{E5A086B8-ED6F-48BC-96DA-310D0A8EDA1E}" name="Titulo " dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{A613DE25-29DE-48D4-BC16-F5717CF7ECA3}" name="Institucion" dataDxfId="105"/>
-    <tableColumn id="4" xr3:uid="{1BDACA12-B245-486A-9E06-9D9098F20E10}" name="Sede" dataDxfId="104"/>
-    <tableColumn id="5" xr3:uid="{D0778336-0469-4990-9EB5-772FE1C892EC}" name="Año" dataDxfId="103"/>
-    <tableColumn id="6" xr3:uid="{2F93E69C-50E8-4280-853E-B1A84DCC7347}" name="Resolucion" dataDxfId="102"/>
-    <tableColumn id="7" xr3:uid="{6460BCE4-0F6E-4660-82BB-1481FEF7B99F}" name="ID Perido" dataDxfId="101"/>
-    <tableColumn id="8" xr3:uid="{6DFD58EC-5274-4E4C-89AE-91FEBF635473}" name="ID Estudiante" dataDxfId="100"/>
+    <tableColumn id="1" xr3:uid="{68514C17-60C3-4A0D-A349-2C66A403B3C1}" name="ID Boletin" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{E5A086B8-ED6F-48BC-96DA-310D0A8EDA1E}" name="Titulo " dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{A613DE25-29DE-48D4-BC16-F5717CF7ECA3}" name="Institucion" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{1BDACA12-B245-486A-9E06-9D9098F20E10}" name="Sede" dataDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{D0778336-0469-4990-9EB5-772FE1C892EC}" name="Año" dataDxfId="108"/>
+    <tableColumn id="6" xr3:uid="{2F93E69C-50E8-4280-853E-B1A84DCC7347}" name="Resolucion" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{6460BCE4-0F6E-4660-82BB-1481FEF7B99F}" name="ID Perido" dataDxfId="106"/>
+    <tableColumn id="8" xr3:uid="{6DFD58EC-5274-4E4C-89AE-91FEBF635473}" name="ID Estudiante" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table67.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="83" xr:uid="{82A6652E-6953-494D-9A75-D898296A7C5E}" name="Tabla6184" displayName="Tabla6184" ref="J46:O49" totalsRowShown="0" headerRowDxfId="99" dataDxfId="97" headerRowBorderDxfId="98" tableBorderDxfId="96" totalsRowBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="83" xr:uid="{82A6652E-6953-494D-9A75-D898296A7C5E}" name="Tabla6184" displayName="Tabla6184" ref="J46:O49" totalsRowShown="0" headerRowDxfId="104" dataDxfId="102" headerRowBorderDxfId="103" tableBorderDxfId="101" totalsRowBorderDxfId="100">
   <autoFilter ref="J46:O49" xr:uid="{82A6652E-6953-494D-9A75-D898296A7C5E}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{97567469-7EC0-47BE-8A0F-5A1E7E4DF284}" name="ID Nota Final" dataDxfId="94"/>
-    <tableColumn id="2" xr3:uid="{95512354-A3A5-4170-91E3-8B55E5A68AE8}" name="Nota Final" dataDxfId="93"/>
-    <tableColumn id="3" xr3:uid="{78209B69-83FF-422E-99F5-164507B288F6}" name="ID Logro" dataDxfId="92"/>
-    <tableColumn id="4" xr3:uid="{2567BA9B-6902-4696-B4E7-685321C8A630}" name="Inasistencias" dataDxfId="91"/>
-    <tableColumn id="5" xr3:uid="{810899C0-1FE2-420A-B918-2FB75D2D4C2D}" name="ID Materia" dataDxfId="90"/>
-    <tableColumn id="6" xr3:uid="{C8BCEDB0-7343-4A37-A004-868A87E54D1E}" name="ID Estudiante" dataDxfId="89"/>
+    <tableColumn id="1" xr3:uid="{97567469-7EC0-47BE-8A0F-5A1E7E4DF284}" name="ID Nota Final" dataDxfId="99"/>
+    <tableColumn id="2" xr3:uid="{95512354-A3A5-4170-91E3-8B55E5A68AE8}" name="Nota Final" dataDxfId="98"/>
+    <tableColumn id="3" xr3:uid="{78209B69-83FF-422E-99F5-164507B288F6}" name="ID Logro" dataDxfId="97"/>
+    <tableColumn id="4" xr3:uid="{2567BA9B-6902-4696-B4E7-685321C8A630}" name="Inasistencias" dataDxfId="96"/>
+    <tableColumn id="5" xr3:uid="{810899C0-1FE2-420A-B918-2FB75D2D4C2D}" name="ID Materia" dataDxfId="95"/>
+    <tableColumn id="6" xr3:uid="{C8BCEDB0-7343-4A37-A004-868A87E54D1E}" name="ID Estudiante" dataDxfId="94"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table68.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="84" xr:uid="{FFFCDFA9-59D7-40DA-8D8C-975DE6209DC9}" name="Tabla6385" displayName="Tabla6385" ref="Q46:R49" totalsRowShown="0" headerRowDxfId="88" dataDxfId="86" headerRowBorderDxfId="87" tableBorderDxfId="85" totalsRowBorderDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="84" xr:uid="{FFFCDFA9-59D7-40DA-8D8C-975DE6209DC9}" name="Tabla6385" displayName="Tabla6385" ref="Q46:R49" totalsRowShown="0" headerRowDxfId="93" dataDxfId="91" headerRowBorderDxfId="92" tableBorderDxfId="90" totalsRowBorderDxfId="89">
   <autoFilter ref="Q46:R49" xr:uid="{FFFCDFA9-59D7-40DA-8D8C-975DE6209DC9}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F97C587C-0CE8-44C9-BFC0-A12C411811E0}" name="ID Logro" dataDxfId="83"/>
-    <tableColumn id="2" xr3:uid="{C89C8218-E38E-4555-9B3A-D2156F8C67E7}" name="Logro" dataDxfId="82"/>
+    <tableColumn id="1" xr3:uid="{F97C587C-0CE8-44C9-BFC0-A12C411811E0}" name="ID Logro" dataDxfId="88"/>
+    <tableColumn id="2" xr3:uid="{C89C8218-E38E-4555-9B3A-D2156F8C67E7}" name="Logro" dataDxfId="87"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table69.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="85" xr:uid="{FA80C4FB-5BE6-471A-80D7-55931BCB5367}" name="Tabla19276686" displayName="Tabla19276686" ref="B67:I70" totalsRowShown="0" headerRowDxfId="81" dataDxfId="79" headerRowBorderDxfId="80" tableBorderDxfId="78" totalsRowBorderDxfId="77">
-  <autoFilter ref="B67:I70" xr:uid="{FA80C4FB-5BE6-471A-80D7-55931BCB5367}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{67181C2E-8654-4208-866E-B4A9EC277C90}" name="ID Noticias" dataDxfId="76"/>
-    <tableColumn id="2" xr3:uid="{EB1ED606-AA85-4CC8-92FD-C6CE175E95A2}" name="Titulo" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{322053DC-2E9C-4A5D-B228-4C95E6159E7E}" name="Descripcion" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{5F0EA3D8-FAFE-437F-8AF0-78DD6F44716F}" name="Fecha" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{ED209CAC-9847-4446-A93B-95D0BD385F9A}" name="ID Tipo" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{8587F818-A980-42BB-9723-AE3E1365AFB7}" name="Imagen 1" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{C8E07683-B419-497E-8412-6AB72EE08442}" name="Imagen 2" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{91A1B327-8C20-44F2-B88D-3F3C00789755}" name="Imagen 3" dataDxfId="69"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="85" xr:uid="{FA80C4FB-5BE6-471A-80D7-55931BCB5367}" name="Tabla19276686" displayName="Tabla19276686" ref="B67:J70" totalsRowShown="0" headerRowDxfId="86" dataDxfId="84" headerRowBorderDxfId="85" tableBorderDxfId="83" totalsRowBorderDxfId="82">
+  <autoFilter ref="B67:J70" xr:uid="{FA80C4FB-5BE6-471A-80D7-55931BCB5367}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{67181C2E-8654-4208-866E-B4A9EC277C90}" name="ID Noticias" dataDxfId="81"/>
+    <tableColumn id="2" xr3:uid="{EB1ED606-AA85-4CC8-92FD-C6CE175E95A2}" name="Titulo" dataDxfId="80"/>
+    <tableColumn id="3" xr3:uid="{322053DC-2E9C-4A5D-B228-4C95E6159E7E}" name="Encabezado" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{5F0EA3D8-FAFE-437F-8AF0-78DD6F44716F}" name="Descripcion1" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{ED209CAC-9847-4446-A93B-95D0BD385F9A}" name="Descripcion2" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{8587F818-A980-42BB-9723-AE3E1365AFB7}" name="Descripcion3" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{C8E07683-B419-497E-8412-6AB72EE08442}" name="Imagen 1" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{91A1B327-8C20-44F2-B88D-3F3C00789755}" name="Imagen 2" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{8106E2BC-A708-4FDE-8916-4CB724493B80}" name="Imagen 3" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{55F88581-5DED-441B-B6FD-007550A5AB83}" name="Tabla22" displayName="Tabla22" ref="B19:G22" totalsRowShown="0" headerRowDxfId="619" dataDxfId="617" headerRowBorderDxfId="618" tableBorderDxfId="616" totalsRowBorderDxfId="615">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{55F88581-5DED-441B-B6FD-007550A5AB83}" name="Tabla22" displayName="Tabla22" ref="B19:G22" totalsRowShown="0" headerRowDxfId="626" dataDxfId="624" headerRowBorderDxfId="625" tableBorderDxfId="623" totalsRowBorderDxfId="622">
   <autoFilter ref="B19:G22" xr:uid="{55F88581-5DED-441B-B6FD-007550A5AB83}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{98B0B63C-DBED-43D8-B1AD-692A73E33F74}" name="ID Usuario" dataDxfId="614"/>
-    <tableColumn id="2" xr3:uid="{00B53C12-D322-4145-9ED3-BB241C7F6744}" name="ID Profesor" dataDxfId="613"/>
-    <tableColumn id="3" xr3:uid="{CAD850A0-530C-476A-B817-1B781B4ED8FF}" name="Tarea" dataDxfId="612"/>
-    <tableColumn id="4" xr3:uid="{CEBD75ED-C476-4E11-B3F3-6D023B273942}" name="Nota" dataDxfId="611"/>
-    <tableColumn id="5" xr3:uid="{11331A03-566A-491B-9557-907993623AD6}" name="Mensage Descripcion" dataDxfId="610"/>
-    <tableColumn id="6" xr3:uid="{4C9BB068-3E2E-494C-88AF-889A306C4C32}" name="Fecha Mensage" dataDxfId="609"/>
+    <tableColumn id="1" xr3:uid="{98B0B63C-DBED-43D8-B1AD-692A73E33F74}" name="ID Usuario" dataDxfId="621"/>
+    <tableColumn id="2" xr3:uid="{00B53C12-D322-4145-9ED3-BB241C7F6744}" name="ID Profesor" dataDxfId="620"/>
+    <tableColumn id="3" xr3:uid="{CAD850A0-530C-476A-B817-1B781B4ED8FF}" name="Tarea" dataDxfId="619"/>
+    <tableColumn id="4" xr3:uid="{CEBD75ED-C476-4E11-B3F3-6D023B273942}" name="Nota" dataDxfId="618"/>
+    <tableColumn id="5" xr3:uid="{11331A03-566A-491B-9557-907993623AD6}" name="Mensage Descripcion" dataDxfId="617"/>
+    <tableColumn id="6" xr3:uid="{4C9BB068-3E2E-494C-88AF-889A306C4C32}" name="Fecha Mensage" dataDxfId="616"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table70.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="86" xr:uid="{C397D472-F2D6-404C-8903-D936293D907E}" name="Tabla336887" displayName="Tabla336887" ref="N67:O71" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65" totalsRowBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="86" xr:uid="{C397D472-F2D6-404C-8903-D936293D907E}" name="Tabla336887" displayName="Tabla336887" ref="N67:O71" totalsRowShown="0" headerRowDxfId="79" dataDxfId="77" headerRowBorderDxfId="78" tableBorderDxfId="76" totalsRowBorderDxfId="75">
   <autoFilter ref="N67:O71" xr:uid="{C397D472-F2D6-404C-8903-D936293D907E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{77374B09-5B19-4E58-AE3F-B9A165F3D73A}" name="ID Valoracion" dataDxfId="63"/>
-    <tableColumn id="2" xr3:uid="{0FB5DD90-5F1B-43EA-A373-3AED87238DCC}" name="Valoracion" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{77374B09-5B19-4E58-AE3F-B9A165F3D73A}" name="ID Valoracion" dataDxfId="74"/>
+    <tableColumn id="2" xr3:uid="{0FB5DD90-5F1B-43EA-A373-3AED87238DCC}" name="Valoracion" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table71.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="87" xr:uid="{ACAD39E3-50E8-40CF-9CB6-9F28F9063ABF}" name="Tabla7988" displayName="Tabla7988" ref="K60:N63" totalsRowShown="0" headerRowDxfId="61" headerRowBorderDxfId="60" tableBorderDxfId="59" totalsRowBorderDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="87" xr:uid="{ACAD39E3-50E8-40CF-9CB6-9F28F9063ABF}" name="Tabla7988" displayName="Tabla7988" ref="K60:N63" totalsRowShown="0" headerRowDxfId="72" headerRowBorderDxfId="71" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <autoFilter ref="K60:N63" xr:uid="{ACAD39E3-50E8-40CF-9CB6-9F28F9063ABF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D3336AFB-BDE7-441F-AB55-A4DB897239A9}" name="ID Boletin Notas" dataDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{356F4CCB-E772-4D6B-9A3E-4DACF79F6C9F}" name="ID Nota Final" dataDxfId="56"/>
-    <tableColumn id="3" xr3:uid="{94C61AE5-AD2A-45C9-B009-358161957B19}" name="ID Valoracion" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{C7304B56-F087-4AC2-884C-B79DD61C06BA}" name="ID Boletin" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{D3336AFB-BDE7-441F-AB55-A4DB897239A9}" name="ID Boletin Notas" dataDxfId="68"/>
+    <tableColumn id="2" xr3:uid="{356F4CCB-E772-4D6B-9A3E-4DACF79F6C9F}" name="ID Nota Final" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{94C61AE5-AD2A-45C9-B009-358161957B19}" name="ID Valoracion" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{C7304B56-F087-4AC2-884C-B79DD61C06BA}" name="ID Boletin" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table72.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="88" xr:uid="{EDE4DF43-8C0B-473C-9FA9-7FC97C625534}" name="Tabla60798189" displayName="Tabla60798189" ref="Q60:U63" totalsRowShown="0" headerRowDxfId="53" dataDxfId="51" headerRowBorderDxfId="52" tableBorderDxfId="50" totalsRowBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="88" xr:uid="{EDE4DF43-8C0B-473C-9FA9-7FC97C625534}" name="Tabla60798189" displayName="Tabla60798189" ref="Q60:U63" totalsRowShown="0" headerRowDxfId="64" dataDxfId="62" headerRowBorderDxfId="63" tableBorderDxfId="61" totalsRowBorderDxfId="60">
   <autoFilter ref="Q60:U63" xr:uid="{EDE4DF43-8C0B-473C-9FA9-7FC97C625534}"/>
   <tableColumns count="5">
-    <tableColumn id="14" xr3:uid="{098B1189-9C1E-4DCE-8247-D57DDF5F5EEA}" name="Puesto" dataDxfId="48"/>
-    <tableColumn id="16" xr3:uid="{DEC01084-ED4F-41F6-82ED-DFA050262101}" name="Comportamiento" dataDxfId="47"/>
-    <tableColumn id="17" xr3:uid="{940AAAA8-113F-4984-86BC-4A24F24928B4}" name="Observaciones" dataDxfId="46"/>
-    <tableColumn id="1" xr3:uid="{20D095C6-1473-49B9-AB21-6028477A2C6A}" name="ID Profesor" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{BAFBC226-5D36-4C18-92BD-BF86E5B8DB11}" name="ID Boletin" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{098B1189-9C1E-4DCE-8247-D57DDF5F5EEA}" name="Puesto" dataDxfId="59"/>
+    <tableColumn id="16" xr3:uid="{DEC01084-ED4F-41F6-82ED-DFA050262101}" name="Comportamiento" dataDxfId="58"/>
+    <tableColumn id="17" xr3:uid="{940AAAA8-113F-4984-86BC-4A24F24928B4}" name="Observaciones" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{20D095C6-1473-49B9-AB21-6028477A2C6A}" name="ID Profesor" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{BAFBC226-5D36-4C18-92BD-BF86E5B8DB11}" name="ID Boletin" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table73.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="89" xr:uid="{752FA8BF-0DFD-417B-806D-097EEB770400}" name="Tabla89" displayName="Tabla89" ref="P60:P63" totalsRowShown="0" headerRowDxfId="43" dataDxfId="41" headerRowBorderDxfId="42" tableBorderDxfId="40" totalsRowBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="89" xr:uid="{752FA8BF-0DFD-417B-806D-097EEB770400}" name="Tabla89" displayName="Tabla89" ref="P60:P63" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51" totalsRowBorderDxfId="50">
   <autoFilter ref="P60:P63" xr:uid="{752FA8BF-0DFD-417B-806D-097EEB770400}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{E0362E2E-D6A8-41D8-BF4E-B3DB6B0699E9}" name="ID Boletin Detalles" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{E0362E2E-D6A8-41D8-BF4E-B3DB6B0699E9}" name="ID Boletin Detalles" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table74.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="91" xr:uid="{2B78F868-2CCC-409C-AE05-7260EE5388F0}" name="Tabla91" displayName="Tabla91" ref="B32:F35" totalsRowShown="0" headerRowDxfId="37" dataDxfId="35" headerRowBorderDxfId="36" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="91" xr:uid="{2B78F868-2CCC-409C-AE05-7260EE5388F0}" name="Tabla91" displayName="Tabla91" ref="B32:F35" totalsRowShown="0" headerRowDxfId="48" dataDxfId="46" headerRowBorderDxfId="47" tableBorderDxfId="45" totalsRowBorderDxfId="44">
   <autoFilter ref="B32:F35" xr:uid="{2B78F868-2CCC-409C-AE05-7260EE5388F0}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4EC6177E-B3F1-461F-8CE7-4AF6ABB3ACC8}" name="ID Aula" dataDxfId="32"/>
-    <tableColumn id="2" xr3:uid="{AB38FE5D-077F-4E53-A52E-3D4BACF6FE71}" name="Nombre Aula" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{4EC9C7DD-CECC-4042-9E43-3627CD8A454B}" name="ID Materia" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{9544E620-7C5A-4576-B622-B9A789B96628}" name="ID Curso" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{0D86CC8F-5839-4C74-AEF7-CF578C5CB905}" name="ID Profesor" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{4EC6177E-B3F1-461F-8CE7-4AF6ABB3ACC8}" name="ID Aula" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{AB38FE5D-077F-4E53-A52E-3D4BACF6FE71}" name="Nombre Aula" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{4EC9C7DD-CECC-4042-9E43-3627CD8A454B}" name="ID Materia" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{9544E620-7C5A-4576-B622-B9A789B96628}" name="ID Curso" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{0D86CC8F-5839-4C74-AEF7-CF578C5CB905}" name="ID Profesor" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table75.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8ED92830-077D-4868-A98F-61C99AE8C6F6}" name="Tabla13" displayName="Tabla13" ref="K67:L70" totalsRowShown="0" headerRowDxfId="27" headerRowBorderDxfId="26" tableBorderDxfId="25" totalsRowBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8ED92830-077D-4868-A98F-61C99AE8C6F6}" name="Tabla13" displayName="Tabla13" ref="K67:L70" totalsRowShown="0" headerRowDxfId="38" headerRowBorderDxfId="37" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="K67:L70" xr:uid="{8ED92830-077D-4868-A98F-61C99AE8C6F6}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{33F57F40-B2E4-4A01-8987-E51FFFD2F808}" name="ID Tipo" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{BD0C0654-D2E6-4977-96C1-C44FF5A982E7}" name="Tipos" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{33F57F40-B2E4-4A01-8987-E51FFFD2F808}" name="Fecha" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{BD0C0654-D2E6-4977-96C1-C44FF5A982E7}" name="ID Tipo" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table76.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{248BB2FF-BC1E-43CD-AB53-C914DC6710B7}" name="Tabla4" displayName="Tabla4" ref="J39:O42" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{248BB2FF-BC1E-43CD-AB53-C914DC6710B7}" name="Tabla4" displayName="Tabla4" ref="J39:O42" totalsRowShown="0" headerRowDxfId="34" dataDxfId="32" headerRowBorderDxfId="33" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="J39:O42" xr:uid="{248BB2FF-BC1E-43CD-AB53-C914DC6710B7}"/>
   <tableColumns count="6">
-    <tableColumn id="3" xr3:uid="{CD3D59E6-3D2A-4449-BDB1-DBD8C2F27CC4}" name="ID comentario" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{22F04B51-D498-4C24-920B-6BF925A899AD}" name="Descripcion" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{A589F8BF-71D3-4F7A-813C-86ABFBDC957C}" name="Fecha" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{FE4B981E-8F9E-487E-BCA3-C1E630A458C5}" name="ID Usuario" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{1B2CE631-3885-4E5B-A9A9-21C23BB57E0A}" name="ID Anuncios" dataDxfId="12"/>
-    <tableColumn id="1" xr3:uid="{54F8B8B7-8EB6-4F59-BEDF-20703A80D069}" name="ID Trabajos" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{CD3D59E6-3D2A-4449-BDB1-DBD8C2F27CC4}" name="ID comentario" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{22F04B51-D498-4C24-920B-6BF925A899AD}" name="Descripcion" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{A589F8BF-71D3-4F7A-813C-86ABFBDC957C}" name="Fecha" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{FE4B981E-8F9E-487E-BCA3-C1E630A458C5}" name="ID Usuario" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{1B2CE631-3885-4E5B-A9A9-21C23BB57E0A}" name="ID Anuncios" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{54F8B8B7-8EB6-4F59-BEDF-20703A80D069}" name="ID Trabajos" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table77.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8E34A65B-8649-4E83-B679-1F1AEBF88E6E}" name="Tabla6" displayName="Tabla6" ref="Q32:U35" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8E34A65B-8649-4E83-B679-1F1AEBF88E6E}" name="Tabla6" displayName="Tabla6" ref="Q32:U35" totalsRowShown="0" headerRowDxfId="23" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20">
   <autoFilter ref="Q32:U35" xr:uid="{8E34A65B-8649-4E83-B679-1F1AEBF88E6E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9AACD995-073C-48E0-BF54-EAA1A16191CC}" name="ID entregados" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{CFDA2296-D0D2-4C2D-B786-4F9C12666FAA}" name="Archivo" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{F5A8004A-31D1-44E4-8337-AA1AE83F1974}" name="Fecha Entrega" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{AC2FB787-C188-4640-811B-827CBA791C93}" name="ID Usuario" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{2F6FCD2A-5E36-456C-AD0E-BDE3CC8E045A}" name="ID Trabajos" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9AACD995-073C-48E0-BF54-EAA1A16191CC}" name="ID entregados" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{CFDA2296-D0D2-4C2D-B786-4F9C12666FAA}" name="Archivo" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{F5A8004A-31D1-44E4-8337-AA1AE83F1974}" name="Fecha Entrega" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{AC2FB787-C188-4640-811B-827CBA791C93}" name="ID Usuario" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{2F6FCD2A-5E36-456C-AD0E-BDE3CC8E045A}" name="ID Trabajos" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table78.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0F17A645-6038-4E0A-980B-32CD12A0CAEB}" name="Tabla134" displayName="Tabla134" ref="B74:C77" totalsRowShown="0" headerRowDxfId="14" headerRowBorderDxfId="12" tableBorderDxfId="13" totalsRowBorderDxfId="11">
+  <autoFilter ref="B74:C77" xr:uid="{0F17A645-6038-4E0A-980B-32CD12A0CAEB}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D82325DD-C5DD-4D81-BD56-43A4CFB87559}" name="ID Tipo" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{408AE6DB-B817-4482-A6A0-26804E1DD3DE}" name="Tipos" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{AB6AAAFC-7EF7-4A75-853E-3103F12DA1ED}" name="Tabla23" displayName="Tabla23" ref="B26:G29" totalsRowShown="0" headerRowDxfId="608" dataDxfId="606" headerRowBorderDxfId="607" tableBorderDxfId="605" totalsRowBorderDxfId="604">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{AB6AAAFC-7EF7-4A75-853E-3103F12DA1ED}" name="Tabla23" displayName="Tabla23" ref="B26:G29" totalsRowShown="0" headerRowDxfId="615" dataDxfId="613" headerRowBorderDxfId="614" tableBorderDxfId="612" totalsRowBorderDxfId="611">
   <autoFilter ref="B26:G29" xr:uid="{AB6AAAFC-7EF7-4A75-853E-3103F12DA1ED}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8172C532-4C1D-4B43-B56B-F6F99D445E51}" name="ID Planilla" dataDxfId="603"/>
-    <tableColumn id="2" xr3:uid="{711461CB-E60D-4049-98B7-79FEEA718907}" name="Nombre Planilla" dataDxfId="602"/>
-    <tableColumn id="3" xr3:uid="{4CFDCD66-4D59-46E3-A25C-AADC5F19E1EF}" name="ID Curso" dataDxfId="601"/>
-    <tableColumn id="4" xr3:uid="{4D447FDD-D6A4-4103-84F2-FD6436828EAC}" name="ID Jornada" dataDxfId="600"/>
-    <tableColumn id="5" xr3:uid="{B2DDACF4-4B10-4E39-B7F5-51B95555D36D}" name="ID Periodo" dataDxfId="599"/>
-    <tableColumn id="6" xr3:uid="{C278B778-7479-4B79-84D6-046499A06B8F}" name="ID Nota Final" dataDxfId="598"/>
+    <tableColumn id="1" xr3:uid="{8172C532-4C1D-4B43-B56B-F6F99D445E51}" name="ID Planilla" dataDxfId="610"/>
+    <tableColumn id="2" xr3:uid="{711461CB-E60D-4049-98B7-79FEEA718907}" name="Nombre Planilla" dataDxfId="609"/>
+    <tableColumn id="3" xr3:uid="{4CFDCD66-4D59-46E3-A25C-AADC5F19E1EF}" name="ID Curso" dataDxfId="608"/>
+    <tableColumn id="4" xr3:uid="{4D447FDD-D6A4-4103-84F2-FD6436828EAC}" name="ID Jornada" dataDxfId="607"/>
+    <tableColumn id="5" xr3:uid="{B2DDACF4-4B10-4E39-B7F5-51B95555D36D}" name="ID Periodo" dataDxfId="606"/>
+    <tableColumn id="6" xr3:uid="{C278B778-7479-4B79-84D6-046499A06B8F}" name="ID Nota Final" dataDxfId="605"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A732164F-1298-4098-B3A5-CA13797F751B}" name="Tabla24" displayName="Tabla24" ref="I19:R22" totalsRowShown="0" headerRowDxfId="597" dataDxfId="595" headerRowBorderDxfId="596" tableBorderDxfId="594" totalsRowBorderDxfId="593">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{A732164F-1298-4098-B3A5-CA13797F751B}" name="Tabla24" displayName="Tabla24" ref="I19:R22" totalsRowShown="0" headerRowDxfId="604" dataDxfId="602" headerRowBorderDxfId="603" tableBorderDxfId="601" totalsRowBorderDxfId="600">
   <autoFilter ref="I19:R22" xr:uid="{A732164F-1298-4098-B3A5-CA13797F751B}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{03D3F956-FACB-470B-BE96-759A218E6468}" name="ID Notas" dataDxfId="592"/>
-    <tableColumn id="2" xr3:uid="{B933BBEB-3FE3-4EDC-8CFC-142DD59E2C9A}" name="Curso" dataDxfId="591"/>
-    <tableColumn id="3" xr3:uid="{FA46C4AA-F666-4692-812A-F9CEE4A84F66}" name="ID Jornada" dataDxfId="590"/>
-    <tableColumn id="4" xr3:uid="{DD6D5824-5566-45E1-B0B6-73520EE036A6}" name="ID Materia " dataDxfId="589"/>
-    <tableColumn id="5" xr3:uid="{DA6D583D-CD6E-4447-96AA-7C8669194889}" name="Nota Final" dataDxfId="588"/>
-    <tableColumn id="6" xr3:uid="{944468B8-4942-4EEC-913E-02AC87CAB576}" name="ID Materia 2" dataDxfId="587"/>
-    <tableColumn id="7" xr3:uid="{1AB07EC7-BD28-43C8-914E-EEEDA218CFAD}" name="Nota Final " dataDxfId="586"/>
-    <tableColumn id="8" xr3:uid="{80B1C153-89E9-4E70-88CA-9B2B34F3DFA8}" name="ID Materia 3" dataDxfId="585"/>
-    <tableColumn id="9" xr3:uid="{7DD9396F-FE7D-47EA-984C-05965D782020}" name="Nota Final2" dataDxfId="584"/>
-    <tableColumn id="10" xr3:uid="{B35E1DDE-FEF6-4220-BFA3-58D49E9280B4}" name="ID Ususario" dataDxfId="583"/>
+    <tableColumn id="1" xr3:uid="{03D3F956-FACB-470B-BE96-759A218E6468}" name="ID Notas" dataDxfId="599"/>
+    <tableColumn id="2" xr3:uid="{B933BBEB-3FE3-4EDC-8CFC-142DD59E2C9A}" name="Curso" dataDxfId="598"/>
+    <tableColumn id="3" xr3:uid="{FA46C4AA-F666-4692-812A-F9CEE4A84F66}" name="ID Jornada" dataDxfId="597"/>
+    <tableColumn id="4" xr3:uid="{DD6D5824-5566-45E1-B0B6-73520EE036A6}" name="ID Materia " dataDxfId="596"/>
+    <tableColumn id="5" xr3:uid="{DA6D583D-CD6E-4447-96AA-7C8669194889}" name="Nota Final" dataDxfId="595"/>
+    <tableColumn id="6" xr3:uid="{944468B8-4942-4EEC-913E-02AC87CAB576}" name="ID Materia 2" dataDxfId="594"/>
+    <tableColumn id="7" xr3:uid="{1AB07EC7-BD28-43C8-914E-EEEDA218CFAD}" name="Nota Final " dataDxfId="593"/>
+    <tableColumn id="8" xr3:uid="{80B1C153-89E9-4E70-88CA-9B2B34F3DFA8}" name="ID Materia 3" dataDxfId="592"/>
+    <tableColumn id="9" xr3:uid="{7DD9396F-FE7D-47EA-984C-05965D782020}" name="Nota Final2" dataDxfId="591"/>
+    <tableColumn id="10" xr3:uid="{B35E1DDE-FEF6-4220-BFA3-58D49E9280B4}" name="ID Ususario" dataDxfId="590"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -24156,10 +24384,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39D037F8-4504-475D-8BB9-A1E9EC6D5669}">
-  <dimension ref="B2:AF72"/>
+  <dimension ref="B2:AF77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26193,9 +26421,7 @@
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
       <c r="J66" s="1"/>
-      <c r="K66" s="132" t="s">
-        <v>329</v>
-      </c>
+      <c r="K66" s="158"/>
       <c r="L66" s="133"/>
       <c r="M66" s="1"/>
       <c r="N66" s="116" t="s">
@@ -26220,29 +26446,31 @@
         <v>77</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>78</v>
+        <v>379</v>
       </c>
       <c r="E67" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J67" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="K67" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F67" s="102" t="s">
+      <c r="L67" s="102" t="s">
         <v>330</v>
-      </c>
-      <c r="G67" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="H67" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="I67" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="J67" s="1"/>
-      <c r="K67" s="102" t="s">
-        <v>330</v>
-      </c>
-      <c r="L67" s="110" t="s">
-        <v>334</v>
       </c>
       <c r="M67" s="1"/>
       <c r="N67" s="102" t="s">
@@ -26271,27 +26499,29 @@
       <c r="D68" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="E68" s="66">
-        <v>45675</v>
-      </c>
-      <c r="F68" s="111" t="s">
-        <v>331</v>
+      <c r="E68" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>36</v>
+        <v>85</v>
       </c>
       <c r="H68" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I68" s="15" t="s">
+      <c r="I68" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J68" s="1"/>
-      <c r="K68" s="111" t="s">
+      <c r="J68" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K68" s="66">
+        <v>45675</v>
+      </c>
+      <c r="L68" s="111" t="s">
         <v>331</v>
-      </c>
-      <c r="L68" s="112" t="s">
-        <v>335</v>
       </c>
       <c r="M68" s="1"/>
       <c r="N68" s="111" t="s">
@@ -26320,27 +26550,29 @@
       <c r="D69" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="E69" s="66">
-        <v>45689</v>
-      </c>
-      <c r="F69" s="111" t="s">
-        <v>332</v>
+      <c r="E69" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="H69" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="I69" s="15" t="s">
+      <c r="I69" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="J69" s="1"/>
-      <c r="K69" s="111" t="s">
+      <c r="J69" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K69" s="66">
+        <v>45689</v>
+      </c>
+      <c r="L69" s="111" t="s">
         <v>332</v>
-      </c>
-      <c r="L69" s="112" t="s">
-        <v>336</v>
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="111" t="s">
@@ -26369,27 +26601,29 @@
       <c r="D70" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E70" s="67">
-        <v>45682</v>
-      </c>
-      <c r="F70" s="113" t="s">
-        <v>333</v>
+      <c r="E70" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>87</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="H70" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="I70" s="21" t="s">
+      <c r="I70" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J70" s="1"/>
-      <c r="K70" s="113" t="s">
+      <c r="J70" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="K70" s="67">
+        <v>45682</v>
+      </c>
+      <c r="L70" s="113" t="s">
         <v>333</v>
-      </c>
-      <c r="L70" s="115" t="s">
-        <v>337</v>
       </c>
       <c r="M70" s="1"/>
       <c r="N70" s="111" t="s">
@@ -26462,6 +26696,44 @@
       <c r="W72" s="1"/>
       <c r="X72" s="1"/>
     </row>
+    <row r="73" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B73" s="132" t="s">
+        <v>329</v>
+      </c>
+      <c r="C73" s="133"/>
+    </row>
+    <row r="74" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B74" s="102" t="s">
+        <v>330</v>
+      </c>
+      <c r="C74" s="110" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="75" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B75" s="111" t="s">
+        <v>331</v>
+      </c>
+      <c r="C75" s="112" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="76" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B76" s="111" t="s">
+        <v>332</v>
+      </c>
+      <c r="C76" s="112" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="77" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B77" s="113" t="s">
+        <v>333</v>
+      </c>
+      <c r="C77" s="115" t="s">
+        <v>337</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -26474,7 +26746,7 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
-  <tableParts count="30">
+  <tableParts count="31">
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
@@ -26505,6 +26777,7 @@
     <tablePart r:id="rId35"/>
     <tablePart r:id="rId36"/>
     <tablePart r:id="rId37"/>
+    <tablePart r:id="rId38"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>